<commit_message>
changed feature files and fixed movie seats
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ExcelData.xlsx
+++ b/src/test/resources/testdata/ExcelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11407" uniqueCount="589">
   <si>
     <t>Start Date</t>
   </si>
@@ -1740,6 +1740,135 @@
   </si>
   <si>
     <t>Japanese</t>
+  </si>
+  <si>
+    <t>2025-08-17T08:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T09:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T11:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T12:30:00</t>
+  </si>
+  <si>
+    <t>2025-09-06T10:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-17T14:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T14:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T09:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-25T16:00:00</t>
+  </si>
+  <si>
+    <t>2025-11-30T16:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T22:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T10:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-02T11:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-26T12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T04:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-17T13:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-30T13:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T08:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T14:00:00</t>
+  </si>
+  <si>
+    <t>Bhaag Milkha Bhaag (2013)</t>
+  </si>
+  <si>
+    <t>Nilgiris: A Shared Wilderness</t>
+  </si>
+  <si>
+    <t>Sarbala Ji</t>
+  </si>
+  <si>
+    <t>Punjabi</t>
+  </si>
+  <si>
+    <t>Sanghavi &amp; Sons</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Telugu</t>
+  </si>
+  <si>
+    <t>Ekka</t>
+  </si>
+  <si>
+    <t>Kannada</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>Nikita Roy</t>
+  </si>
+  <si>
+    <t>Murderbaad</t>
+  </si>
+  <si>
+    <t>26 Sep - 2 Oct, 5:30PM</t>
+  </si>
+  <si>
+    <t>18 Jul - 17 Aug, 9AM</t>
+  </si>
+  <si>
+    <t>17 Jul - 17 Aug, 9AM</t>
+  </si>
+  <si>
+    <t>26 Jul - 27 Jul, 10AM</t>
+  </si>
+  <si>
+    <t>26 Sep - 28 Sep, 5:30PM</t>
+  </si>
+  <si>
+    <t>18 Jul - 18 Aug, 9AM</t>
+  </si>
+  <si>
+    <t>2025-07-18T11:00:00</t>
   </si>
 </sst>
 </file>
@@ -2145,7 +2274,7 @@
         <v>439</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>431</v>
+        <v>546</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>5</v>
@@ -2159,10 +2288,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>432</v>
+        <v>547</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>433</v>
+        <v>458</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>7</v>
@@ -2196,7 +2325,7 @@
         <v>443</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>437</v>
+        <v>548</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>11</v>
@@ -2230,7 +2359,7 @@
         <v>432</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>433</v>
+        <v>458</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>15</v>
@@ -2244,10 +2373,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>431</v>
+        <v>549</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>16</v>
@@ -2346,10 +2475,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>437</v>
+        <v>548</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>27</v>
@@ -2363,7 +2492,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="B15" t="s" s="0">
         <v>438</v>
@@ -2380,10 +2509,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>447</v>
+        <v>549</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>31</v>
@@ -2400,7 +2529,7 @@
         <v>539</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>540</v>
+        <v>550</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>33</v>
@@ -2434,7 +2563,7 @@
         <v>451</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>452</v>
+        <v>551</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>37</v>
@@ -2465,7 +2594,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B21" t="s" s="0">
         <v>438</v>
@@ -2482,10 +2611,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>455</v>
+        <v>552</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>456</v>
+        <v>553</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>43</v>
@@ -2499,10 +2628,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>455</v>
+        <v>554</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>457</v>
+        <v>555</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>45</v>
@@ -2516,10 +2645,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>432</v>
+        <v>547</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>458</v>
+        <v>556</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>47</v>
@@ -2536,7 +2665,7 @@
         <v>432</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>433</v>
+        <v>458</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>49</v>
@@ -2587,7 +2716,7 @@
         <v>443</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>437</v>
+        <v>548</v>
       </c>
       <c r="C28" t="s" s="0">
         <v>52</v>
@@ -2621,7 +2750,7 @@
         <v>441</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>447</v>
+        <v>549</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>55</v>
@@ -2635,10 +2764,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>455</v>
+        <v>554</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>56</v>
@@ -2652,10 +2781,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>463</v>
+        <v>557</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>435</v>
+        <v>558</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>58</v>
@@ -2706,7 +2835,7 @@
         <v>441</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>447</v>
+        <v>549</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>64</v>
@@ -2723,7 +2852,7 @@
         <v>441</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>447</v>
+        <v>549</v>
       </c>
       <c r="C36" t="s" s="0">
         <v>65</v>
@@ -2771,7 +2900,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="B39" t="s" s="0">
         <v>438</v>
@@ -2805,7 +2934,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>466</v>
+        <v>559</v>
       </c>
       <c r="B41" t="s" s="0">
         <v>473</v>
@@ -2876,7 +3005,7 @@
         <v>464</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>78</v>
@@ -2890,10 +3019,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>464</v>
+        <v>560</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>465</v>
+        <v>561</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>80</v>
@@ -2924,10 +3053,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
+        <v>562</v>
+      </c>
+      <c r="B48" t="s" s="0">
         <v>478</v>
-      </c>
-      <c r="B48" t="s" s="0">
-        <v>435</v>
       </c>
       <c r="C48" t="s" s="0">
         <v>84</v>
@@ -2944,7 +3073,7 @@
         <v>443</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>437</v>
+        <v>548</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>86</v>
@@ -2958,10 +3087,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>447</v>
+        <v>549</v>
       </c>
       <c r="C50" t="s" s="0">
         <v>88</v>
@@ -2975,10 +3104,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
+        <v>563</v>
+      </c>
+      <c r="B51" t="s" s="0">
         <v>479</v>
-      </c>
-      <c r="B51" t="s" s="0">
-        <v>435</v>
       </c>
       <c r="C51" t="s" s="0">
         <v>89</v>
@@ -3083,7 +3212,7 @@
         <v>481</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D57" t="s" s="0">
         <v>92</v>
@@ -3100,7 +3229,7 @@
         <v>481</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D58" t="s" s="0">
         <v>92</v>
@@ -3117,7 +3246,7 @@
         <v>481</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" t="s" s="0">
         <v>92</v>
@@ -3145,13 +3274,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D61" t="s" s="0">
         <v>102</v>
@@ -3162,13 +3291,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D62" t="s" s="0">
         <v>102</v>
@@ -3179,10 +3308,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
+        <v>437</v>
+      </c>
+      <c r="B63" t="s" s="0">
         <v>488</v>
-      </c>
-      <c r="B63" t="s" s="0">
-        <v>435</v>
       </c>
       <c r="C63" t="s" s="0">
         <v>104</v>
@@ -3196,7 +3325,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B64" t="s" s="0">
         <v>438</v>
@@ -3230,7 +3359,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B66" t="s" s="0">
         <v>438</v>
@@ -3247,13 +3376,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>474</v>
+        <v>490</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>475</v>
+        <v>491</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D67" t="s" s="0">
         <v>76</v>
@@ -3270,7 +3399,7 @@
         <v>475</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D68" t="s" s="0">
         <v>76</v>
@@ -3281,13 +3410,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B69" t="s" s="0">
         <v>475</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D69" t="s" s="0">
         <v>76</v>
@@ -3298,13 +3427,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s" s="0">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D70" t="s" s="0">
         <v>76</v>
@@ -3315,13 +3444,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s" s="0">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="B71" t="s" s="0">
         <v>475</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D71" t="s" s="0">
         <v>76</v>
@@ -3338,7 +3467,7 @@
         <v>481</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s" s="0">
         <v>92</v>
@@ -3355,7 +3484,7 @@
         <v>481</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D73" t="s" s="0">
         <v>92</v>
@@ -3372,7 +3501,7 @@
         <v>481</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D74" t="s" s="0">
         <v>92</v>
@@ -3389,7 +3518,7 @@
         <v>481</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D75" t="s" s="0">
         <v>92</v>
@@ -3406,7 +3535,7 @@
         <v>481</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D76" t="s" s="0">
         <v>92</v>
@@ -3423,7 +3552,7 @@
         <v>481</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D77" t="s" s="0">
         <v>92</v>
@@ -3440,7 +3569,7 @@
         <v>481</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D78" t="s" s="0">
         <v>92</v>
@@ -3457,7 +3586,7 @@
         <v>481</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D79" t="s" s="0">
         <v>92</v>
@@ -3474,7 +3603,7 @@
         <v>481</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D80" t="s" s="0">
         <v>92</v>
@@ -3491,7 +3620,7 @@
         <v>481</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D81" t="s" s="0">
         <v>92</v>
@@ -3525,7 +3654,7 @@
         <v>481</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D83" t="s" s="0">
         <v>92</v>
@@ -3542,7 +3671,7 @@
         <v>481</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D84" t="s" s="0">
         <v>92</v>
@@ -3559,7 +3688,7 @@
         <v>481</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D85" t="s" s="0">
         <v>92</v>
@@ -3593,7 +3722,7 @@
         <v>481</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D87" t="s" s="0">
         <v>92</v>
@@ -3610,7 +3739,7 @@
         <v>481</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D88" t="s" s="0">
         <v>92</v>
@@ -3627,7 +3756,7 @@
         <v>481</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D89" t="s" s="0">
         <v>92</v>
@@ -3644,7 +3773,7 @@
         <v>474</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D90" t="s" s="0">
         <v>94</v>
@@ -3658,10 +3787,10 @@
         <v>480</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="D91" t="s" s="0">
         <v>94</v>
@@ -3678,7 +3807,7 @@
         <v>474</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D92" t="s" s="0">
         <v>94</v>
@@ -3695,7 +3824,7 @@
         <v>474</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D93" t="s" s="0">
         <v>94</v>
@@ -3712,7 +3841,7 @@
         <v>474</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D94" t="s" s="0">
         <v>94</v>
@@ -3726,10 +3855,10 @@
         <v>480</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D95" t="s" s="0">
         <v>94</v>
@@ -3746,7 +3875,7 @@
         <v>474</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D96" t="s" s="0">
         <v>94</v>
@@ -3760,7 +3889,7 @@
         <v>541</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>493</v>
+        <v>564</v>
       </c>
       <c r="C97" t="s" s="0">
         <v>494</v>
@@ -3879,10 +4008,10 @@
         <v>476</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>501</v>
+        <v>477</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D104" t="s" s="0">
         <v>154</v>
@@ -3896,10 +4025,10 @@
         <v>476</v>
       </c>
       <c r="B105" t="s" s="0">
-        <v>477</v>
+        <v>501</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D105" t="s" s="0">
         <v>154</v>
@@ -3961,13 +4090,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s" s="0">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="B109" t="s" s="0">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D109" t="s" s="0">
         <v>163</v>
@@ -3978,13 +4107,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s" s="0">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B110" t="s" s="0">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C110" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D110" t="s" s="0">
         <v>163</v>
@@ -4120,7 +4249,7 @@
         <v>481</v>
       </c>
       <c r="C118" t="s" s="0">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D118" t="s" s="0">
         <v>92</v>
@@ -4137,7 +4266,7 @@
         <v>481</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D119" t="s" s="0">
         <v>92</v>
@@ -4154,7 +4283,7 @@
         <v>481</v>
       </c>
       <c r="C120" t="s" s="0">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D120" t="s" s="0">
         <v>92</v>
@@ -4171,7 +4300,7 @@
         <v>481</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D121" t="s" s="0">
         <v>92</v>
@@ -4188,7 +4317,7 @@
         <v>481</v>
       </c>
       <c r="C122" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D122" t="s" s="0">
         <v>92</v>
@@ -4205,7 +4334,7 @@
         <v>481</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D123" t="s" s="0">
         <v>92</v>
@@ -4222,7 +4351,7 @@
         <v>474</v>
       </c>
       <c r="C124" t="s" s="0">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D124" t="s" s="0">
         <v>94</v>
@@ -4239,7 +4368,7 @@
         <v>474</v>
       </c>
       <c r="C125" t="s" s="0">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D125" t="s" s="0">
         <v>94</v>
@@ -4250,10 +4379,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s" s="0">
-        <v>443</v>
+        <v>565</v>
       </c>
       <c r="B126" t="s" s="0">
-        <v>514</v>
+        <v>566</v>
       </c>
       <c r="C126" t="s" s="0">
         <v>183</v>
@@ -4403,10 +4532,10 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s" s="0">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B135" t="s" s="0">
-        <v>447</v>
+        <v>549</v>
       </c>
       <c r="C135" t="s" s="0">
         <v>197</v>
@@ -4420,10 +4549,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s" s="0">
-        <v>439</v>
+        <v>567</v>
       </c>
       <c r="B136" t="s" s="0">
-        <v>431</v>
+        <v>546</v>
       </c>
       <c r="C136" t="s" s="0">
         <v>199</v>
@@ -4698,7 +4827,7 @@
         <v>481</v>
       </c>
       <c r="C152" t="s" s="0">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D152" t="s" s="0">
         <v>92</v>
@@ -4749,7 +4878,7 @@
         <v>481</v>
       </c>
       <c r="C155" t="s" s="0">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D155" t="s" s="0">
         <v>92</v>
@@ -4780,7 +4909,7 @@
         <v>532</v>
       </c>
       <c r="B157" t="s" s="0">
-        <v>533</v>
+        <v>568</v>
       </c>
       <c r="C157" t="s" s="0">
         <v>228</v>
@@ -4893,7 +5022,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>246</v>
+        <v>582</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>247</v>
@@ -4921,10 +5050,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>251</v>
@@ -4935,10 +5064,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>409</v>
+        <v>249</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>410</v>
+        <v>254</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>251</v>
@@ -4949,10 +5078,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>252</v>
+        <v>409</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>253</v>
+        <v>410</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>251</v>
@@ -4977,13 +5106,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D13" t="n" s="0">
         <v>100.0</v>
@@ -4991,13 +5120,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D14" t="n" s="0">
         <v>100.0</v>
@@ -5005,13 +5134,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D15" t="n" s="0">
         <v>100.0</v>
@@ -5019,13 +5148,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D16" t="n" s="0">
         <v>100.0</v>
@@ -5033,27 +5162,27 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>270</v>
+        <v>536</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>100.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>536</v>
+        <v>275</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D18" t="n" s="0">
         <v>149.0</v>
@@ -5061,16 +5190,16 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>149.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -5089,27 +5218,27 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>278</v>
+        <v>583</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="D21" t="n" s="0">
-        <v>150.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>282</v>
+        <v>584</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>284</v>
+        <v>8</v>
       </c>
       <c r="D22" t="n" s="0">
         <v>168.0</v>
@@ -5117,13 +5246,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>282</v>
+        <v>583</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="D23" t="n" s="0">
         <v>168.0</v>
@@ -5131,24 +5260,24 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>282</v>
+        <v>537</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D24" t="n" s="0">
-        <v>168.0</v>
+        <v>169.0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>537</v>
+        <v>241</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>289</v>
@@ -5159,10 +5288,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>241</v>
+        <v>280</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>289</v>
@@ -5173,13 +5302,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D27" t="n" s="0">
         <v>169.0</v>
@@ -5187,13 +5316,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>264</v>
+        <v>294</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D28" t="n" s="0">
         <v>169.0</v>
@@ -5201,44 +5330,44 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D29" t="n" s="0">
-        <v>169.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
-        <v>297</v>
+        <v>583</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>299</v>
+        <v>8</v>
       </c>
       <c r="D30" t="n" s="0">
-        <v>179.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>8</v>
+        <v>302</v>
       </c>
       <c r="D31" t="n" s="0">
-        <v>198.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -5246,10 +5375,10 @@
         <v>255</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="D32" t="n" s="0">
         <v>199.0</v>
@@ -5257,13 +5386,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s" s="0">
-        <v>255</v>
+        <v>585</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>257</v>
+        <v>306</v>
       </c>
       <c r="D33" t="n" s="0">
         <v>199.0</v>
@@ -5271,13 +5400,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D34" t="n" s="0">
         <v>199.0</v>
@@ -5285,13 +5414,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="D35" t="n" s="0">
         <v>199.0</v>
@@ -5299,13 +5428,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D36" t="n" s="0">
         <v>199.0</v>
@@ -5313,27 +5442,27 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>234</v>
+        <v>316</v>
       </c>
       <c r="D37" t="n" s="0">
-        <v>199.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D38" t="n" s="0">
         <v>200.0</v>
@@ -5341,41 +5470,41 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>264</v>
+        <v>319</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D39" t="n" s="0">
-        <v>200.0</v>
+        <v>219.0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="D40" t="n" s="0">
-        <v>219.0</v>
+        <v>249.0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>274</v>
+        <v>105</v>
       </c>
       <c r="D41" t="n" s="0">
         <v>249.0</v>
@@ -5383,13 +5512,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>324</v>
+        <v>586</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>325</v>
+        <v>247</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>105</v>
+        <v>327</v>
       </c>
       <c r="D42" t="n" s="0">
         <v>249.0</v>
@@ -5397,41 +5526,41 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>247</v>
+        <v>329</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D43" t="n" s="0">
-        <v>249.0</v>
+        <v>270.0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s" s="0">
-        <v>328</v>
+        <v>241</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>329</v>
+        <v>411</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>330</v>
+        <v>412</v>
       </c>
       <c r="D44" t="n" s="0">
-        <v>270.0</v>
+        <v>299.0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s" s="0">
-        <v>241</v>
+        <v>331</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>411</v>
+        <v>332</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>412</v>
+        <v>274</v>
       </c>
       <c r="D45" t="n" s="0">
         <v>299.0</v>
@@ -5439,27 +5568,27 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>331</v>
+        <v>538</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>274</v>
+        <v>227</v>
       </c>
       <c r="D46" t="n" s="0">
-        <v>299.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>538</v>
+        <v>334</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>227</v>
+        <v>277</v>
       </c>
       <c r="D47" t="n" s="0">
         <v>300.0</v>
@@ -5467,55 +5596,55 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>277</v>
+        <v>330</v>
       </c>
       <c r="D48" t="n" s="0">
-        <v>300.0</v>
+        <v>320.0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s" s="0">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>330</v>
+        <v>277</v>
       </c>
       <c r="D49" t="n" s="0">
-        <v>320.0</v>
+        <v>349.0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D50" t="n" s="0">
-        <v>349.0</v>
+        <v>399.0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="D51" t="n" s="0">
         <v>399.0</v>
@@ -5523,16 +5652,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>318</v>
+        <v>345</v>
       </c>
       <c r="D52" t="n" s="0">
-        <v>399.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -5540,7 +5669,7 @@
         <v>343</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C53" t="s" s="0">
         <v>345</v>
@@ -5565,55 +5694,55 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s" s="0">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>345</v>
+        <v>277</v>
       </c>
       <c r="D55" t="n" s="0">
-        <v>450.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>348</v>
+        <v>426</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>349</v>
+        <v>427</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>277</v>
+        <v>428</v>
       </c>
       <c r="D56" t="n" s="0">
-        <v>499.0</v>
+        <v>599.0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s" s="0">
-        <v>426</v>
+        <v>350</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>427</v>
+        <v>351</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>428</v>
+        <v>352</v>
       </c>
       <c r="D57" t="n" s="0">
-        <v>599.0</v>
+        <v>999.0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s" s="0">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D58" t="n" s="0">
         <v>999.0</v>
@@ -5621,24 +5750,24 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
-        <v>353</v>
+        <v>421</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>354</v>
+        <v>422</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>355</v>
+        <v>237</v>
       </c>
       <c r="D59" t="n" s="0">
-        <v>999.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s" s="0">
-        <v>421</v>
+        <v>356</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>422</v>
+        <v>357</v>
       </c>
       <c r="C60" t="s" s="0">
         <v>237</v>
@@ -5649,13 +5778,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>237</v>
+        <v>360</v>
       </c>
       <c r="D61" t="n" s="0">
         <v>1000.0</v>
@@ -5663,100 +5792,100 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>358</v>
+        <v>587</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>360</v>
+        <v>216</v>
       </c>
       <c r="D62" t="n" s="0">
-        <v>1000.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>429</v>
+        <v>362</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>216</v>
+        <v>364</v>
       </c>
       <c r="D63" t="n" s="0">
-        <v>1200.0</v>
+        <v>1499.0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>362</v>
+        <v>264</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>364</v>
+        <v>296</v>
       </c>
       <c r="D64" t="n" s="0">
-        <v>1499.0</v>
+        <v>1999.0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>264</v>
+        <v>366</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>296</v>
+        <v>216</v>
       </c>
       <c r="D65" t="n" s="0">
-        <v>1999.0</v>
+        <v>2010.0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>366</v>
+        <v>423</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>216</v>
+        <v>369</v>
       </c>
       <c r="D66" t="n" s="0">
-        <v>2010.0</v>
+        <v>3000.0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>423</v>
+        <v>370</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D67" t="n" s="0">
-        <v>3000.0</v>
+        <v>5000.0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="D68" t="n" s="0">
-        <v>5000.0</v>
+        <v>6499.0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -5780,7 +5909,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -5801,7 +5930,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>383</v>
@@ -5812,7 +5941,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>383</v>
@@ -5823,24 +5952,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>380</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>380</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -5889,21 +6018,21 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>392</v>
+        <v>569</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>383</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>384</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>384</v>
@@ -5911,13 +6040,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>534</v>
+        <v>393</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>394</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -5966,7 +6095,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>535</v>
+        <v>570</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>380</v>
@@ -5977,21 +6106,21 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>543</v>
+        <v>571</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>383</v>
+        <v>572</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>545</v>
+        <v>394</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>381</v>
@@ -5999,67 +6128,144 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>399</v>
+        <v>575</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>380</v>
+        <v>576</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>400</v>
+        <v>573</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>401</v>
+        <v>574</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>384</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>402</v>
+        <v>577</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>383</v>
+        <v>578</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>403</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>404</v>
+        <v>580</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>406</v>
+        <v>380</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>397</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
+        <v>581</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>383</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>543</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>383</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>400</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>401</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>535</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>380</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>544</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>545</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>405</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>406</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
         <v>407</v>
       </c>
-      <c r="B25" t="s" s="0">
+      <c r="B31" t="s" s="0">
         <v>401</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C31" t="s" s="0">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>407</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>401</v>
+      </c>
+      <c r="C32" t="s" s="0">
         <v>408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Screenshot and logs added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ExcelData.xlsx
+++ b/src/test/resources/testdata/ExcelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11407" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19398" uniqueCount="611">
   <si>
     <t>Start Date</t>
   </si>
@@ -1869,6 +1869,72 @@
   </si>
   <si>
     <t>2025-07-18T11:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-27T16:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-12T16:00:00</t>
+  </si>
+  <si>
+    <t>1-1 Guidance on Stock market By SEBI Registered Entity For Free. Whatsapp on +919702914863</t>
+  </si>
+  <si>
+    <t>Pune, undefined</t>
+  </si>
+  <si>
+    <t>2025-07-17T16:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T16:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-30T15:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T15:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T14:00:00</t>
+  </si>
+  <si>
+    <t>24 Jul, 1PM</t>
+  </si>
+  <si>
+    <t>2025-07-17T17:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-30T17:00:00</t>
+  </si>
+  <si>
+    <t>18 Jul - 20 Jul, 5PM</t>
+  </si>
+  <si>
+    <t>Ba Da BNTR - Korean Food Pop-Up</t>
+  </si>
+  <si>
+    <t>BNTR Taproof, Pune</t>
+  </si>
+  <si>
+    <t>2025-07-17T16:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T16:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-17T15:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T15:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T15:00:00</t>
+  </si>
+  <si>
+    <t>27 Sep - 28 Sep, 4PM</t>
+  </si>
+  <si>
+    <t>Rock N Dhol Shubharambh – Pune's Biggest Disco Dandiya Festival | Navratri 2025</t>
   </si>
 </sst>
 </file>
@@ -2244,7 +2310,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E157"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2271,70 +2337,70 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>439</v>
+        <v>589</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>546</v>
+        <v>590</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>591</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>6</v>
+        <v>592</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>547</v>
+        <v>439</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>458</v>
+        <v>546</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>99.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>434</v>
+        <v>547</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>150.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>548</v>
+        <v>435</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>175.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2342,98 +2408,98 @@
         <v>443</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>438</v>
+        <v>548</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>189.0</v>
+        <v>175.0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>458</v>
+        <v>438</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>198.0</v>
+        <v>189.0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>549</v>
+        <v>458</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>200.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>440</v>
+        <v>604</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>435</v>
+        <v>605</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>250.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>290.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="n" s="0">
         <v>290.0</v>
@@ -2441,50 +2507,50 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>299.0</v>
+        <v>290.0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B13" t="s" s="0">
         <v>435</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>300.0</v>
+        <v>299.0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>548</v>
+        <v>435</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" t="n" s="0">
         <v>300.0</v>
@@ -2495,81 +2561,81 @@
         <v>443</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>438</v>
+        <v>548</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>325.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>549</v>
+        <v>438</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>350.0</v>
+        <v>325.0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>539</v>
+        <v>441</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>475.0</v>
+        <v>350.0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>450</v>
+        <v>606</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>435</v>
+        <v>607</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E18" t="n" s="0">
-        <v>499.0</v>
+        <v>475.0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>551</v>
+        <v>435</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" t="n" s="0">
         <v>499.0</v>
@@ -2577,16 +2643,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>454</v>
+        <v>551</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" t="n" s="0">
         <v>499.0</v>
@@ -2594,33 +2660,33 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>588</v>
+        <v>608</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" t="n" s="0">
-        <v>500.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>552</v>
+        <v>588</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>553</v>
+        <v>438</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" t="n" s="0">
         <v>500.0</v>
@@ -2628,33 +2694,33 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>554</v>
+        <v>593</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>555</v>
+        <v>594</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" t="n" s="0">
-        <v>540.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E24" t="n" s="0">
         <v>540.0</v>
@@ -2662,16 +2728,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>432</v>
+        <v>547</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>458</v>
+        <v>556</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E25" t="n" s="0">
         <v>540.0</v>
@@ -2679,67 +2745,67 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>459</v>
+        <v>432</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>460</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>318</v>
+        <v>8</v>
       </c>
       <c r="E26" t="n" s="0">
-        <v>550.0</v>
+        <v>540.0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>462</v>
+        <v>435</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>50</v>
+        <v>460</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>51</v>
+        <v>318</v>
       </c>
       <c r="E27" t="n" s="0">
-        <v>599.0</v>
+        <v>550.0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>443</v>
+        <v>461</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>548</v>
+        <v>462</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E28" t="n" s="0">
-        <v>600.0</v>
+        <v>599.0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>435</v>
+        <v>548</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E29" t="n" s="0">
         <v>600.0</v>
@@ -2747,16 +2813,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>549</v>
+        <v>435</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E30" t="n" s="0">
         <v>600.0</v>
@@ -2764,16 +2830,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>554</v>
+        <v>441</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>457</v>
+        <v>549</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E31" t="n" s="0">
         <v>600.0</v>
@@ -2781,16 +2847,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>558</v>
+        <v>457</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E32" t="n" s="0">
         <v>600.0</v>
@@ -2798,53 +2864,53 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s" s="0">
-        <v>464</v>
+        <v>557</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>465</v>
+        <v>558</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E33" t="n" s="0">
-        <v>619.0</v>
+        <v>600.0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>466</v>
+        <v>560</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>435</v>
+        <v>561</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" t="n" s="0">
-        <v>699.0</v>
+        <v>619.0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
-        <v>441</v>
+        <v>466</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>549</v>
+        <v>435</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="E35" t="n" s="0">
-        <v>700.0</v>
+        <v>699.0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -2855,78 +2921,78 @@
         <v>549</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="E36" t="n" s="0">
-        <v>720.0</v>
+        <v>700.0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>465</v>
+        <v>549</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E37" t="n" s="0">
-        <v>743.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>467</v>
+        <v>560</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>468</v>
+        <v>561</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E38" t="n" s="0">
-        <v>750.0</v>
+        <v>743.0</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>443</v>
+        <v>467</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>438</v>
+        <v>468</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="E39" t="n" s="0">
-        <v>799.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>470</v>
+        <v>438</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>471</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>472</v>
+        <v>30</v>
       </c>
       <c r="E40" t="n" s="0">
         <v>799.0</v>
@@ -2934,16 +3000,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>559</v>
+        <v>469</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>71</v>
+        <v>471</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>72</v>
+        <v>472</v>
       </c>
       <c r="E41" t="n" s="0">
         <v>799.0</v>
@@ -2951,36 +3017,36 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>467</v>
+        <v>559</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E42" t="n" s="0">
-        <v>850.0</v>
+        <v>799.0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E43" t="n" s="0">
-        <v>899.0</v>
+        <v>850.0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -2991,7 +3057,7 @@
         <v>475</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D44" t="s" s="0">
         <v>76</v>
@@ -3002,16 +3068,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s" s="0">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E45" t="n" s="0">
         <v>899.0</v>
@@ -3019,67 +3085,67 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>560</v>
+        <v>464</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>561</v>
+        <v>465</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E46" t="n" s="0">
-        <v>942.0</v>
+        <v>899.0</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>476</v>
+        <v>560</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>477</v>
+        <v>561</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E47" t="n" s="0">
-        <v>999.0</v>
+        <v>942.0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>562</v>
+        <v>476</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E48" t="n" s="0">
-        <v>1000.0</v>
+        <v>999.0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s" s="0">
-        <v>443</v>
+        <v>562</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>548</v>
+        <v>478</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E49" t="n" s="0">
         <v>1000.0</v>
@@ -3087,16 +3153,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="E50" t="n" s="0">
         <v>1000.0</v>
@@ -3104,36 +3170,36 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>563</v>
+        <v>441</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>479</v>
+        <v>549</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="E51" t="n" s="0">
-        <v>1050.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s" s="0">
-        <v>480</v>
+        <v>563</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E52" t="n" s="0">
-        <v>1099.0</v>
+        <v>1050.0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -3144,7 +3210,7 @@
         <v>481</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D53" t="s" s="0">
         <v>92</v>
@@ -3158,13 +3224,13 @@
         <v>480</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E54" t="n" s="0">
         <v>1099.0</v>
@@ -3172,50 +3238,50 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s" s="0">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E55" t="n" s="0">
-        <v>1100.0</v>
+        <v>1099.0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="E56" t="n" s="0">
-        <v>1199.0</v>
+        <v>1100.0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E57" t="n" s="0">
         <v>1199.0</v>
@@ -3229,7 +3295,7 @@
         <v>481</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D58" t="s" s="0">
         <v>92</v>
@@ -3246,7 +3312,7 @@
         <v>481</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D59" t="s" s="0">
         <v>92</v>
@@ -3260,13 +3326,13 @@
         <v>480</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E60" t="n" s="0">
         <v>1199.0</v>
@@ -3274,19 +3340,19 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E61" t="n" s="0">
-        <v>1200.0</v>
+        <v>1199.0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -3308,16 +3374,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>437</v>
+        <v>484</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E63" t="n" s="0">
         <v>1200.0</v>
@@ -3325,16 +3391,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>588</v>
+        <v>437</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E64" t="n" s="0">
         <v>1200.0</v>
@@ -3342,16 +3408,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>489</v>
+        <v>588</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E65" t="n" s="0">
         <v>1200.0</v>
@@ -3359,16 +3425,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>588</v>
+        <v>489</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E66" t="n" s="0">
         <v>1200.0</v>
@@ -3376,19 +3442,19 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>490</v>
+        <v>588</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>491</v>
+        <v>438</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="E67" t="n" s="0">
-        <v>1299.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -3399,7 +3465,7 @@
         <v>475</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D68" t="s" s="0">
         <v>76</v>
@@ -3416,7 +3482,7 @@
         <v>475</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D69" t="s" s="0">
         <v>76</v>
@@ -3433,7 +3499,7 @@
         <v>475</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D70" t="s" s="0">
         <v>76</v>
@@ -3461,16 +3527,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s" s="0">
-        <v>480</v>
+        <v>490</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E72" t="n" s="0">
         <v>1299.0</v>
@@ -3484,7 +3550,7 @@
         <v>481</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D73" t="s" s="0">
         <v>92</v>
@@ -3501,7 +3567,7 @@
         <v>481</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D74" t="s" s="0">
         <v>92</v>
@@ -3518,7 +3584,7 @@
         <v>481</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D75" t="s" s="0">
         <v>92</v>
@@ -3535,7 +3601,7 @@
         <v>481</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D76" t="s" s="0">
         <v>92</v>
@@ -3552,7 +3618,7 @@
         <v>481</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D77" t="s" s="0">
         <v>92</v>
@@ -3569,7 +3635,7 @@
         <v>481</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D78" t="s" s="0">
         <v>92</v>
@@ -3586,7 +3652,7 @@
         <v>481</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D79" t="s" s="0">
         <v>92</v>
@@ -3603,7 +3669,7 @@
         <v>481</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D80" t="s" s="0">
         <v>92</v>
@@ -3637,7 +3703,7 @@
         <v>481</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D82" t="s" s="0">
         <v>92</v>
@@ -3654,7 +3720,7 @@
         <v>481</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D83" t="s" s="0">
         <v>92</v>
@@ -3671,7 +3737,7 @@
         <v>481</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D84" t="s" s="0">
         <v>92</v>
@@ -3688,7 +3754,7 @@
         <v>481</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D85" t="s" s="0">
         <v>92</v>
@@ -3705,7 +3771,7 @@
         <v>481</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D86" t="s" s="0">
         <v>92</v>
@@ -3722,7 +3788,7 @@
         <v>481</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D87" t="s" s="0">
         <v>92</v>
@@ -3739,7 +3805,7 @@
         <v>481</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D88" t="s" s="0">
         <v>92</v>
@@ -3756,7 +3822,7 @@
         <v>481</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D89" t="s" s="0">
         <v>92</v>
@@ -3770,13 +3836,13 @@
         <v>480</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D90" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E90" t="n" s="0">
         <v>1299.0</v>
@@ -3790,7 +3856,7 @@
         <v>474</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="D91" t="s" s="0">
         <v>94</v>
@@ -3807,7 +3873,7 @@
         <v>474</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="D92" t="s" s="0">
         <v>94</v>
@@ -3821,10 +3887,10 @@
         <v>480</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D93" t="s" s="0">
         <v>94</v>
@@ -3841,7 +3907,7 @@
         <v>474</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D94" t="s" s="0">
         <v>94</v>
@@ -3855,10 +3921,10 @@
         <v>480</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D95" t="s" s="0">
         <v>94</v>
@@ -3875,7 +3941,7 @@
         <v>474</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D96" t="s" s="0">
         <v>94</v>
@@ -3886,36 +3952,36 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s" s="0">
-        <v>541</v>
+        <v>480</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>564</v>
+        <v>474</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>494</v>
+        <v>135</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>495</v>
+        <v>94</v>
       </c>
       <c r="E97" t="n" s="0">
-        <v>1300.0</v>
+        <v>1299.0</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s" s="0">
-        <v>476</v>
+        <v>541</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>496</v>
+        <v>564</v>
       </c>
       <c r="C98" t="s" s="0">
-        <v>141</v>
+        <v>494</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>142</v>
+        <v>495</v>
       </c>
       <c r="E98" t="n" s="0">
-        <v>1399.0</v>
+        <v>1300.0</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
@@ -3926,10 +3992,10 @@
         <v>496</v>
       </c>
       <c r="C99" t="s" s="0">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E99" t="n" s="0">
         <v>1399.0</v>
@@ -3937,16 +4003,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s" s="0">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="B100" t="s" s="0">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E100" t="n" s="0">
         <v>1399.0</v>
@@ -3954,16 +4020,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s" s="0">
-        <v>476</v>
+        <v>497</v>
       </c>
       <c r="B101" t="s" s="0">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D101" t="s" s="0">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E101" t="n" s="0">
         <v>1399.0</v>
@@ -3971,33 +4037,33 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s" s="0">
-        <v>499</v>
+        <v>476</v>
       </c>
       <c r="B102" t="s" s="0">
-        <v>435</v>
+        <v>496</v>
       </c>
       <c r="C102" t="s" s="0">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D102" t="s" s="0">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E102" t="n" s="0">
-        <v>1400.0</v>
+        <v>1399.0</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s" s="0">
-        <v>476</v>
+        <v>499</v>
       </c>
       <c r="B103" t="s" s="0">
-        <v>500</v>
+        <v>435</v>
       </c>
       <c r="C103" t="s" s="0">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D103" t="s" s="0">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E103" t="n" s="0">
         <v>1400.0</v>
@@ -4008,13 +4074,13 @@
         <v>476</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>477</v>
+        <v>500</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D104" t="s" s="0">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E104" t="n" s="0">
         <v>1400.0</v>
@@ -4039,19 +4105,19 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s" s="0">
-        <v>502</v>
+        <v>476</v>
       </c>
       <c r="B106" t="s" s="0">
-        <v>503</v>
+        <v>477</v>
       </c>
       <c r="C106" t="s" s="0">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D106" t="s" s="0">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E106" t="n" s="0">
-        <v>1449.0</v>
+        <v>1400.0</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
@@ -4062,10 +4128,10 @@
         <v>503</v>
       </c>
       <c r="C107" t="s" s="0">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D107" t="s" s="0">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E107" t="n" s="0">
         <v>1449.0</v>
@@ -4073,16 +4139,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s" s="0">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B108" t="s" s="0">
         <v>503</v>
       </c>
       <c r="C108" t="s" s="0">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D108" t="s" s="0">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E108" t="n" s="0">
         <v>1449.0</v>
@@ -4090,30 +4156,30 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s" s="0">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B109" t="s" s="0">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D109" t="s" s="0">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E109" t="n" s="0">
-        <v>1450.0</v>
+        <v>1449.0</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s" s="0">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="B110" t="s" s="0">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C110" t="s" s="0">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D110" t="s" s="0">
         <v>163</v>
@@ -4124,16 +4190,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s" s="0">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="B111" t="s" s="0">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D111" t="s" s="0">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E111" t="n" s="0">
         <v>1450.0</v>
@@ -4141,16 +4207,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s" s="0">
-        <v>476</v>
+        <v>508</v>
       </c>
       <c r="B112" t="s" s="0">
-        <v>501</v>
+        <v>509</v>
       </c>
       <c r="C112" t="s" s="0">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D112" t="s" s="0">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E112" t="n" s="0">
         <v>1450.0</v>
@@ -4158,16 +4224,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s" s="0">
-        <v>512</v>
+        <v>476</v>
       </c>
       <c r="B113" t="s" s="0">
-        <v>477</v>
+        <v>501</v>
       </c>
       <c r="C113" t="s" s="0">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D113" t="s" s="0">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="E113" t="n" s="0">
         <v>1450.0</v>
@@ -4209,16 +4275,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s" s="0">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B116" t="s" s="0">
-        <v>435</v>
+        <v>477</v>
       </c>
       <c r="C116" t="s" s="0">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D116" t="s" s="0">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="E116" t="n" s="0">
         <v>1450.0</v>
@@ -4226,33 +4292,33 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s" s="0">
-        <v>474</v>
+        <v>513</v>
       </c>
       <c r="B117" t="s" s="0">
-        <v>475</v>
+        <v>435</v>
       </c>
       <c r="C117" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D117" t="s" s="0">
-        <v>76</v>
+        <v>173</v>
       </c>
       <c r="E117" t="n" s="0">
-        <v>1499.0</v>
+        <v>1450.0</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B118" t="s" s="0">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C118" t="s" s="0">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D118" t="s" s="0">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E118" t="n" s="0">
         <v>1499.0</v>
@@ -4266,7 +4332,7 @@
         <v>481</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D119" t="s" s="0">
         <v>92</v>
@@ -4283,7 +4349,7 @@
         <v>481</v>
       </c>
       <c r="C120" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D120" t="s" s="0">
         <v>92</v>
@@ -4300,7 +4366,7 @@
         <v>481</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D121" t="s" s="0">
         <v>92</v>
@@ -4317,7 +4383,7 @@
         <v>481</v>
       </c>
       <c r="C122" t="s" s="0">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D122" t="s" s="0">
         <v>92</v>
@@ -4348,13 +4414,13 @@
         <v>480</v>
       </c>
       <c r="B124" t="s" s="0">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C124" t="s" s="0">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D124" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E124" t="n" s="0">
         <v>1499.0</v>
@@ -4379,16 +4445,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s" s="0">
-        <v>565</v>
+        <v>480</v>
       </c>
       <c r="B126" t="s" s="0">
-        <v>566</v>
+        <v>474</v>
       </c>
       <c r="C126" t="s" s="0">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D126" t="s" s="0">
-        <v>184</v>
+        <v>94</v>
       </c>
       <c r="E126" t="n" s="0">
         <v>1499.0</v>
@@ -4396,16 +4462,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s" s="0">
-        <v>515</v>
+        <v>599</v>
       </c>
       <c r="B127" t="s" s="0">
-        <v>516</v>
+        <v>600</v>
       </c>
       <c r="C127" t="s" s="0">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D127" t="s" s="0">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E127" t="n" s="0">
         <v>1499.0</v>
@@ -4413,16 +4479,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s" s="0">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B128" t="s" s="0">
-        <v>503</v>
+        <v>516</v>
       </c>
       <c r="C128" t="s" s="0">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D128" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E128" t="n" s="0">
         <v>1499.0</v>
@@ -4430,16 +4496,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s" s="0">
-        <v>476</v>
+        <v>517</v>
       </c>
       <c r="B129" t="s" s="0">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="C129" t="s" s="0">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D129" t="s" s="0">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E129" t="n" s="0">
         <v>1499.0</v>
@@ -4447,16 +4513,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s" s="0">
-        <v>515</v>
+        <v>476</v>
       </c>
       <c r="B130" t="s" s="0">
-        <v>516</v>
+        <v>496</v>
       </c>
       <c r="C130" t="s" s="0">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D130" t="s" s="0">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="E130" t="n" s="0">
         <v>1499.0</v>
@@ -4464,16 +4530,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s" s="0">
-        <v>476</v>
+        <v>515</v>
       </c>
       <c r="B131" t="s" s="0">
-        <v>496</v>
+        <v>516</v>
       </c>
       <c r="C131" t="s" s="0">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D131" t="s" s="0">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="E131" t="n" s="0">
         <v>1499.0</v>
@@ -4481,16 +4547,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s" s="0">
-        <v>518</v>
+        <v>476</v>
       </c>
       <c r="B132" t="s" s="0">
-        <v>519</v>
+        <v>496</v>
       </c>
       <c r="C132" t="s" s="0">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D132" t="s" s="0">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="E132" t="n" s="0">
         <v>1499.0</v>
@@ -4498,24 +4564,24 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s" s="0">
-        <v>490</v>
+        <v>518</v>
       </c>
       <c r="B133" t="s" s="0">
-        <v>435</v>
+        <v>519</v>
       </c>
       <c r="C133" t="s" s="0">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D133" t="s" s="0">
-        <v>196</v>
+        <v>63</v>
       </c>
       <c r="E133" t="n" s="0">
-        <v>1500.0</v>
+        <v>1499.0</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s" s="0">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B134" t="s" s="0">
         <v>435</v>
@@ -4524,7 +4590,7 @@
         <v>195</v>
       </c>
       <c r="D134" t="s" s="0">
-        <v>105</v>
+        <v>196</v>
       </c>
       <c r="E134" t="n" s="0">
         <v>1500.0</v>
@@ -4532,16 +4598,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s" s="0">
-        <v>441</v>
+        <v>491</v>
       </c>
       <c r="B135" t="s" s="0">
-        <v>549</v>
+        <v>435</v>
       </c>
       <c r="C135" t="s" s="0">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D135" t="s" s="0">
-        <v>198</v>
+        <v>105</v>
       </c>
       <c r="E135" t="n" s="0">
         <v>1500.0</v>
@@ -4549,16 +4615,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s" s="0">
-        <v>567</v>
+        <v>441</v>
       </c>
       <c r="B136" t="s" s="0">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C136" t="s" s="0">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D136" t="s" s="0">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E136" t="n" s="0">
         <v>1500.0</v>
@@ -4566,87 +4632,87 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s" s="0">
-        <v>518</v>
+        <v>567</v>
       </c>
       <c r="B137" t="s" s="0">
-        <v>519</v>
+        <v>546</v>
       </c>
       <c r="C137" t="s" s="0">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D137" t="s" s="0">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E137" t="n" s="0">
-        <v>1549.0</v>
+        <v>1500.0</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s" s="0">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>435</v>
+        <v>519</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D138" t="s" s="0">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="E138" t="n" s="0">
-        <v>1550.0</v>
+        <v>1549.0</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s" s="0">
-        <v>476</v>
+        <v>520</v>
       </c>
       <c r="B139" t="s" s="0">
-        <v>496</v>
+        <v>435</v>
       </c>
       <c r="C139" t="s" s="0">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D139" t="s" s="0">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="E139" t="n" s="0">
-        <v>1559.0</v>
+        <v>1550.0</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s" s="0">
-        <v>443</v>
+        <v>476</v>
       </c>
       <c r="B140" t="s" s="0">
-        <v>521</v>
+        <v>496</v>
       </c>
       <c r="C140" t="s" s="0">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D140" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E140" t="n" s="0">
-        <v>1660.0</v>
+        <v>1559.0</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s" s="0">
-        <v>480</v>
+        <v>443</v>
       </c>
       <c r="B141" t="s" s="0">
-        <v>481</v>
+        <v>521</v>
       </c>
       <c r="C141" t="s" s="0">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D141" t="s" s="0">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="E141" t="n" s="0">
-        <v>1699.0</v>
+        <v>1660.0</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -4657,7 +4723,7 @@
         <v>481</v>
       </c>
       <c r="C142" t="s" s="0">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D142" t="s" s="0">
         <v>92</v>
@@ -4671,13 +4737,13 @@
         <v>480</v>
       </c>
       <c r="B143" t="s" s="0">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C143" t="s" s="0">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D143" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E143" t="n" s="0">
         <v>1699.0</v>
@@ -4685,16 +4751,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s" s="0">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="B144" t="s" s="0">
-        <v>519</v>
+        <v>474</v>
       </c>
       <c r="C144" t="s" s="0">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D144" t="s" s="0">
-        <v>212</v>
+        <v>94</v>
       </c>
       <c r="E144" t="n" s="0">
         <v>1699.0</v>
@@ -4702,67 +4768,67 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s" s="0">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B145" t="s" s="0">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="C145" t="s" s="0">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D145" t="s" s="0">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E145" t="n" s="0">
-        <v>1700.0</v>
+        <v>1699.0</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s" s="0">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B146" t="s" s="0">
-        <v>435</v>
+        <v>524</v>
       </c>
       <c r="C146" t="s" s="0">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D146" t="s" s="0">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E146" t="n" s="0">
-        <v>1770.0</v>
+        <v>1700.0</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s" s="0">
-        <v>480</v>
+        <v>525</v>
       </c>
       <c r="B147" t="s" s="0">
-        <v>481</v>
+        <v>435</v>
       </c>
       <c r="C147" t="s" s="0">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D147" t="s" s="0">
-        <v>92</v>
+        <v>216</v>
       </c>
       <c r="E147" t="n" s="0">
-        <v>1799.0</v>
+        <v>1770.0</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s" s="0">
-        <v>526</v>
+        <v>480</v>
       </c>
       <c r="B148" t="s" s="0">
-        <v>527</v>
+        <v>481</v>
       </c>
       <c r="C148" t="s" s="0">
-        <v>528</v>
+        <v>217</v>
       </c>
       <c r="D148" t="s" s="0">
-        <v>529</v>
+        <v>92</v>
       </c>
       <c r="E148" t="n" s="0">
         <v>1799.0</v>
@@ -4770,50 +4836,50 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s" s="0">
-        <v>499</v>
+        <v>526</v>
       </c>
       <c r="B149" t="s" s="0">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C149" t="s" s="0">
-        <v>218</v>
+        <v>528</v>
       </c>
       <c r="D149" t="s" s="0">
-        <v>219</v>
+        <v>529</v>
       </c>
       <c r="E149" t="n" s="0">
-        <v>2100.0</v>
+        <v>1799.0</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s" s="0">
-        <v>474</v>
+        <v>499</v>
       </c>
       <c r="B150" t="s" s="0">
-        <v>475</v>
+        <v>530</v>
       </c>
       <c r="C150" t="s" s="0">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D150" t="s" s="0">
-        <v>76</v>
+        <v>219</v>
       </c>
       <c r="E150" t="n" s="0">
-        <v>2299.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B151" t="s" s="0">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C151" t="s" s="0">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D151" t="s" s="0">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E151" t="n" s="0">
         <v>2299.0</v>
@@ -4827,13 +4893,13 @@
         <v>481</v>
       </c>
       <c r="C152" t="s" s="0">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D152" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E152" t="n" s="0">
-        <v>2499.0</v>
+        <v>2299.0</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
@@ -4889,35 +4955,52 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s" s="0">
-        <v>531</v>
+        <v>480</v>
       </c>
       <c r="B156" t="s" s="0">
-        <v>435</v>
+        <v>481</v>
       </c>
       <c r="C156" t="s" s="0">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D156" t="s" s="0">
-        <v>227</v>
+        <v>92</v>
       </c>
       <c r="E156" t="n" s="0">
-        <v>2950.0</v>
+        <v>2499.0</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s" s="0">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B157" t="s" s="0">
+        <v>435</v>
+      </c>
+      <c r="C157" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="D157" t="s" s="0">
+        <v>227</v>
+      </c>
+      <c r="E157" t="n" s="0">
+        <v>2950.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="0">
+        <v>597</v>
+      </c>
+      <c r="B158" t="s" s="0">
         <v>568</v>
       </c>
-      <c r="C157" t="s" s="0">
+      <c r="C158" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="D157" t="s" s="0">
+      <c r="D158" t="s" s="0">
         <v>229</v>
       </c>
-      <c r="E157" t="n" s="0">
+      <c r="E158" t="n" s="0">
         <v>3000.0</v>
       </c>
     </row>
@@ -4928,7 +5011,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -4980,30 +5063,30 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>238</v>
+        <v>601</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>239</v>
+        <v>602</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>240</v>
+        <v>603</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>49.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -5022,13 +5105,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>582</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D7" t="n" s="0">
         <v>49.0</v>
@@ -5036,24 +5119,24 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>249</v>
+        <v>582</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>99.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>251</v>
@@ -5092,13 +5175,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D12" t="n" s="0">
         <v>99.0</v>
@@ -5106,27 +5189,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>100.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>264</v>
+        <v>598</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D14" t="n" s="0">
         <v>100.0</v>
@@ -5134,13 +5217,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D15" t="n" s="0">
         <v>100.0</v>
@@ -5148,13 +5231,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D16" t="n" s="0">
         <v>100.0</v>
@@ -5162,86 +5245,86 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>536</v>
+        <v>267</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>149.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>149.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>278</v>
+        <v>536</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>150.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>150.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>583</v>
+        <v>280</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="D21" t="n" s="0">
-        <v>168.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>584</v>
+        <v>278</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>8</v>
+        <v>251</v>
       </c>
       <c r="D22" t="n" s="0">
-        <v>168.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -5249,10 +5332,10 @@
         <v>583</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D23" t="n" s="0">
         <v>168.0</v>
@@ -5260,38 +5343,38 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>537</v>
+        <v>584</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>289</v>
+        <v>8</v>
       </c>
       <c r="D24" t="n" s="0">
-        <v>169.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>241</v>
+        <v>583</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D25" t="n" s="0">
-        <v>169.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>280</v>
+        <v>537</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>289</v>
@@ -5302,13 +5385,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D27" t="n" s="0">
         <v>169.0</v>
@@ -5316,13 +5399,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D28" t="n" s="0">
         <v>169.0</v>
@@ -5330,69 +5413,69 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>297</v>
+        <v>264</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D29" t="n" s="0">
-        <v>179.0</v>
+        <v>169.0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
-        <v>583</v>
+        <v>294</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>8</v>
+        <v>296</v>
       </c>
       <c r="D30" t="n" s="0">
-        <v>198.0</v>
+        <v>169.0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D31" t="n" s="0">
-        <v>199.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>255</v>
+        <v>583</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>257</v>
+        <v>8</v>
       </c>
       <c r="D32" t="n" s="0">
-        <v>199.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s" s="0">
-        <v>585</v>
+        <v>255</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D33" t="n" s="0">
         <v>199.0</v>
@@ -5400,13 +5483,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>307</v>
+        <v>255</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>309</v>
+        <v>257</v>
       </c>
       <c r="D34" t="n" s="0">
         <v>199.0</v>
@@ -5414,13 +5497,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
-        <v>310</v>
+        <v>585</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>240</v>
+        <v>306</v>
       </c>
       <c r="D35" t="n" s="0">
         <v>199.0</v>
@@ -5428,13 +5511,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="D36" t="n" s="0">
         <v>199.0</v>
@@ -5442,27 +5525,27 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>316</v>
+        <v>240</v>
       </c>
       <c r="D37" t="n" s="0">
-        <v>200.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D38" t="n" s="0">
         <v>200.0</v>
@@ -5470,41 +5553,41 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>319</v>
+        <v>264</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D39" t="n" s="0">
-        <v>219.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>274</v>
+        <v>321</v>
       </c>
       <c r="D40" t="n" s="0">
-        <v>249.0</v>
+        <v>219.0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>105</v>
+        <v>274</v>
       </c>
       <c r="D41" t="n" s="0">
         <v>249.0</v>
@@ -5512,13 +5595,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>586</v>
+        <v>324</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>247</v>
+        <v>325</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>327</v>
+        <v>105</v>
       </c>
       <c r="D42" t="n" s="0">
         <v>249.0</v>
@@ -5526,41 +5609,41 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>328</v>
+        <v>586</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>329</v>
+        <v>247</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D43" t="n" s="0">
-        <v>270.0</v>
+        <v>249.0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s" s="0">
-        <v>241</v>
+        <v>328</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>411</v>
+        <v>329</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>412</v>
+        <v>330</v>
       </c>
       <c r="D44" t="n" s="0">
-        <v>299.0</v>
+        <v>270.0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s" s="0">
-        <v>331</v>
+        <v>241</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>332</v>
+        <v>411</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>274</v>
+        <v>412</v>
       </c>
       <c r="D45" t="n" s="0">
         <v>299.0</v>
@@ -5568,27 +5651,27 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>538</v>
+        <v>331</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>227</v>
+        <v>274</v>
       </c>
       <c r="D46" t="n" s="0">
-        <v>300.0</v>
+        <v>299.0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>334</v>
+        <v>538</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>277</v>
+        <v>227</v>
       </c>
       <c r="D47" t="n" s="0">
         <v>300.0</v>
@@ -5596,55 +5679,55 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>330</v>
+        <v>277</v>
       </c>
       <c r="D48" t="n" s="0">
-        <v>320.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s" s="0">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>277</v>
+        <v>330</v>
       </c>
       <c r="D49" t="n" s="0">
-        <v>349.0</v>
+        <v>320.0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D50" t="n" s="0">
-        <v>399.0</v>
+        <v>349.0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>318</v>
+        <v>274</v>
       </c>
       <c r="D51" t="n" s="0">
         <v>399.0</v>
@@ -5652,16 +5735,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s" s="0">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="D52" t="n" s="0">
-        <v>450.0</v>
+        <v>399.0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -5669,7 +5752,7 @@
         <v>343</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C53" t="s" s="0">
         <v>345</v>
@@ -5694,97 +5777,97 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s" s="0">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>277</v>
+        <v>345</v>
       </c>
       <c r="D55" t="n" s="0">
-        <v>499.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>426</v>
+        <v>609</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>427</v>
+        <v>610</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>428</v>
+        <v>364</v>
       </c>
       <c r="D56" t="n" s="0">
-        <v>599.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s" s="0">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>352</v>
+        <v>277</v>
       </c>
       <c r="D57" t="n" s="0">
-        <v>999.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s" s="0">
-        <v>353</v>
+        <v>426</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>354</v>
+        <v>427</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>355</v>
+        <v>428</v>
       </c>
       <c r="D58" t="n" s="0">
-        <v>999.0</v>
+        <v>599.0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
-        <v>421</v>
+        <v>350</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>422</v>
+        <v>351</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>237</v>
+        <v>352</v>
       </c>
       <c r="D59" t="n" s="0">
-        <v>1000.0</v>
+        <v>999.0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s" s="0">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>237</v>
+        <v>355</v>
       </c>
       <c r="D60" t="n" s="0">
-        <v>1000.0</v>
+        <v>999.0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>358</v>
+        <v>421</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>359</v>
+        <v>422</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>360</v>
+        <v>237</v>
       </c>
       <c r="D61" t="n" s="0">
         <v>1000.0</v>
@@ -5792,113 +5875,127 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>587</v>
+        <v>356</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="D62" t="n" s="0">
-        <v>1200.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D63" t="n" s="0">
-        <v>1499.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>264</v>
+        <v>587</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>296</v>
+        <v>216</v>
       </c>
       <c r="D64" t="n" s="0">
-        <v>1999.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>216</v>
+        <v>364</v>
       </c>
       <c r="D65" t="n" s="0">
-        <v>2010.0</v>
+        <v>1499.0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>423</v>
+        <v>264</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>369</v>
+        <v>296</v>
       </c>
       <c r="D66" t="n" s="0">
-        <v>3000.0</v>
+        <v>1999.0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>372</v>
+        <v>216</v>
       </c>
       <c r="D67" t="n" s="0">
-        <v>5000.0</v>
+        <v>2010.0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>373</v>
+        <v>423</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D68" t="n" s="0">
-        <v>6499.0</v>
+        <v>3000.0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s" s="0">
+        <v>370</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>371</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="D69" t="n" s="0">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="B69" t="s" s="0">
+      <c r="B70" t="s" s="0">
         <v>374</v>
       </c>
-      <c r="C69" t="s" s="0">
+      <c r="C70" t="s" s="0">
         <v>375</v>
       </c>
-      <c r="D69" t="n" s="0">
+      <c r="D70" t="n" s="0">
         <v>6499.0</v>
       </c>
     </row>
@@ -5941,10 +6038,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>384</v>
@@ -5952,10 +6049,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>384</v>
@@ -6018,21 +6115,21 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>569</v>
+        <v>392</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>383</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>403</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>384</v>
@@ -6040,13 +6137,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>393</v>
+        <v>580</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -6062,123 +6159,123 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>395</v>
+        <v>569</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>389</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>398</v>
+        <v>534</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>542</v>
+        <v>400</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>383</v>
+        <v>401</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>403</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>380</v>
+        <v>576</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>571</v>
+        <v>399</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>572</v>
+        <v>380</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>534</v>
+        <v>543</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>381</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>573</v>
+        <v>535</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>574</v>
+        <v>380</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>578</v>
+        <v>380</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>384</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>580</v>
+        <v>542</v>
       </c>
       <c r="B23" t="s" s="0">
         <v>383</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>381</v>
+        <v>403</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>399</v>
+        <v>544</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>380</v>
+        <v>545</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25">
@@ -6194,57 +6291,57 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>543</v>
+        <v>571</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>383</v>
+        <v>572</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>384</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>535</v>
+        <v>407</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>380</v>
+        <v>401</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>544</v>
+        <v>573</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>545</v>
+        <v>574</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>381</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>397</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
Validated contact form and did some bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ExcelData.xlsx
+++ b/src/test/resources/testdata/ExcelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23100" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25971" uniqueCount="699">
   <si>
     <t>Start Date</t>
   </si>
@@ -2172,6 +2172,33 @@
   </si>
   <si>
     <t>Azamgarh</t>
+  </si>
+  <si>
+    <t>2025-07-17T18:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T18:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T17:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-17T17:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T17:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-31T21:00:00</t>
+  </si>
+  <si>
+    <t>Harishchandragad Trek by e2e</t>
+  </si>
+  <si>
+    <t>Harishchandra fort, Pune</t>
+  </si>
+  <si>
+    <t>Waterfall Hike</t>
   </si>
 </sst>
 </file>
@@ -2547,7 +2574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2693,10 +2720,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>604</v>
+        <v>690</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>605</v>
+        <v>691</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>16</v>
@@ -2846,10 +2873,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>604</v>
+        <v>690</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>605</v>
+        <v>691</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>33</v>
@@ -3294,7 +3321,7 @@
         <v>475</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s" s="0">
         <v>76</v>
@@ -3311,7 +3338,7 @@
         <v>475</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s" s="0">
         <v>76</v>
@@ -3719,7 +3746,7 @@
         <v>475</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D69" t="s" s="0">
         <v>76</v>
@@ -3730,13 +3757,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s" s="0">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="B70" t="s" s="0">
         <v>475</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D70" t="s" s="0">
         <v>76</v>
@@ -3747,13 +3774,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B71" t="s" s="0">
         <v>475</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D71" t="s" s="0">
         <v>76</v>
@@ -3770,7 +3797,7 @@
         <v>475</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D72" t="s" s="0">
         <v>76</v>
@@ -3787,7 +3814,7 @@
         <v>481</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D73" t="s" s="0">
         <v>92</v>
@@ -3804,7 +3831,7 @@
         <v>481</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D74" t="s" s="0">
         <v>92</v>
@@ -3821,7 +3848,7 @@
         <v>481</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D75" t="s" s="0">
         <v>92</v>
@@ -3838,7 +3865,7 @@
         <v>481</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D76" t="s" s="0">
         <v>92</v>
@@ -3855,7 +3882,7 @@
         <v>481</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D77" t="s" s="0">
         <v>92</v>
@@ -3872,7 +3899,7 @@
         <v>481</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D78" t="s" s="0">
         <v>92</v>
@@ -3889,7 +3916,7 @@
         <v>481</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D79" t="s" s="0">
         <v>92</v>
@@ -3906,7 +3933,7 @@
         <v>481</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D80" t="s" s="0">
         <v>92</v>
@@ -3923,7 +3950,7 @@
         <v>481</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D81" t="s" s="0">
         <v>92</v>
@@ -3940,7 +3967,7 @@
         <v>481</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D82" t="s" s="0">
         <v>92</v>
@@ -3957,7 +3984,7 @@
         <v>481</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D83" t="s" s="0">
         <v>92</v>
@@ -3974,7 +4001,7 @@
         <v>481</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D84" t="s" s="0">
         <v>92</v>
@@ -3991,7 +4018,7 @@
         <v>481</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="D85" t="s" s="0">
         <v>92</v>
@@ -4008,7 +4035,7 @@
         <v>481</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D86" t="s" s="0">
         <v>92</v>
@@ -4025,7 +4052,7 @@
         <v>481</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D87" t="s" s="0">
         <v>92</v>
@@ -4042,7 +4069,7 @@
         <v>481</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D88" t="s" s="0">
         <v>92</v>
@@ -4059,7 +4086,7 @@
         <v>481</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D89" t="s" s="0">
         <v>92</v>
@@ -4076,7 +4103,7 @@
         <v>481</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D90" t="s" s="0">
         <v>92</v>
@@ -4090,10 +4117,10 @@
         <v>480</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D91" t="s" s="0">
         <v>94</v>
@@ -4110,7 +4137,7 @@
         <v>474</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D92" t="s" s="0">
         <v>94</v>
@@ -4144,7 +4171,7 @@
         <v>474</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="D94" t="s" s="0">
         <v>94</v>
@@ -4161,7 +4188,7 @@
         <v>474</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D95" t="s" s="0">
         <v>94</v>
@@ -4178,7 +4205,7 @@
         <v>474</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D96" t="s" s="0">
         <v>94</v>
@@ -4192,10 +4219,10 @@
         <v>480</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="D97" t="s" s="0">
         <v>94</v>
@@ -4478,13 +4505,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s" s="0">
-        <v>512</v>
+        <v>476</v>
       </c>
       <c r="B114" t="s" s="0">
-        <v>477</v>
+        <v>501</v>
       </c>
       <c r="C114" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D114" t="s" s="0">
         <v>154</v>
@@ -4495,13 +4522,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s" s="0">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B115" t="s" s="0">
-        <v>511</v>
+        <v>477</v>
       </c>
       <c r="C115" t="s" s="0">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D115" t="s" s="0">
         <v>154</v>
@@ -4512,13 +4539,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s" s="0">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="B116" t="s" s="0">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="C116" t="s" s="0">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D116" t="s" s="0">
         <v>154</v>
@@ -4569,7 +4596,7 @@
         <v>481</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D119" t="s" s="0">
         <v>92</v>
@@ -4603,7 +4630,7 @@
         <v>481</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D121" t="s" s="0">
         <v>92</v>
@@ -4620,7 +4647,7 @@
         <v>481</v>
       </c>
       <c r="C122" t="s" s="0">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D122" t="s" s="0">
         <v>92</v>
@@ -4637,7 +4664,7 @@
         <v>481</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D123" t="s" s="0">
         <v>92</v>
@@ -4699,10 +4726,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s" s="0">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="B127" t="s" s="0">
-        <v>600</v>
+        <v>514</v>
       </c>
       <c r="C127" t="s" s="0">
         <v>183</v>
@@ -4818,24 +4845,24 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s" s="0">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="B134" t="s" s="0">
-        <v>435</v>
+        <v>695</v>
       </c>
       <c r="C134" t="s" s="0">
-        <v>195</v>
+        <v>696</v>
       </c>
       <c r="D134" t="s" s="0">
-        <v>196</v>
+        <v>697</v>
       </c>
       <c r="E134" t="n" s="0">
-        <v>1500.0</v>
+        <v>1499.0</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s" s="0">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B135" t="s" s="0">
         <v>435</v>
@@ -4844,7 +4871,7 @@
         <v>195</v>
       </c>
       <c r="D135" t="s" s="0">
-        <v>105</v>
+        <v>196</v>
       </c>
       <c r="E135" t="n" s="0">
         <v>1500.0</v>
@@ -4852,16 +4879,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s" s="0">
-        <v>441</v>
+        <v>491</v>
       </c>
       <c r="B136" t="s" s="0">
-        <v>549</v>
+        <v>435</v>
       </c>
       <c r="C136" t="s" s="0">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D136" t="s" s="0">
-        <v>198</v>
+        <v>105</v>
       </c>
       <c r="E136" t="n" s="0">
         <v>1500.0</v>
@@ -4869,16 +4896,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s" s="0">
-        <v>567</v>
+        <v>441</v>
       </c>
       <c r="B137" t="s" s="0">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C137" t="s" s="0">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D137" t="s" s="0">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E137" t="n" s="0">
         <v>1500.0</v>
@@ -4886,87 +4913,87 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s" s="0">
-        <v>518</v>
+        <v>567</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>519</v>
+        <v>546</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D138" t="s" s="0">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E138" t="n" s="0">
-        <v>1549.0</v>
+        <v>1500.0</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s" s="0">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B139" t="s" s="0">
-        <v>435</v>
+        <v>519</v>
       </c>
       <c r="C139" t="s" s="0">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D139" t="s" s="0">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="E139" t="n" s="0">
-        <v>1550.0</v>
+        <v>1549.0</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s" s="0">
-        <v>476</v>
+        <v>520</v>
       </c>
       <c r="B140" t="s" s="0">
-        <v>496</v>
+        <v>435</v>
       </c>
       <c r="C140" t="s" s="0">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D140" t="s" s="0">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="E140" t="n" s="0">
-        <v>1559.0</v>
+        <v>1550.0</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s" s="0">
-        <v>443</v>
+        <v>476</v>
       </c>
       <c r="B141" t="s" s="0">
-        <v>521</v>
+        <v>496</v>
       </c>
       <c r="C141" t="s" s="0">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D141" t="s" s="0">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E141" t="n" s="0">
-        <v>1660.0</v>
+        <v>1559.0</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s" s="0">
-        <v>480</v>
+        <v>443</v>
       </c>
       <c r="B142" t="s" s="0">
-        <v>481</v>
+        <v>521</v>
       </c>
       <c r="C142" t="s" s="0">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D142" t="s" s="0">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="E142" t="n" s="0">
-        <v>1699.0</v>
+        <v>1660.0</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
@@ -4991,13 +5018,13 @@
         <v>480</v>
       </c>
       <c r="B144" t="s" s="0">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C144" t="s" s="0">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D144" t="s" s="0">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E144" t="n" s="0">
         <v>1699.0</v>
@@ -5005,16 +5032,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s" s="0">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="B145" t="s" s="0">
-        <v>519</v>
+        <v>474</v>
       </c>
       <c r="C145" t="s" s="0">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D145" t="s" s="0">
-        <v>212</v>
+        <v>94</v>
       </c>
       <c r="E145" t="n" s="0">
         <v>1699.0</v>
@@ -5022,67 +5049,67 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s" s="0">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B146" t="s" s="0">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="C146" t="s" s="0">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D146" t="s" s="0">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E146" t="n" s="0">
-        <v>1700.0</v>
+        <v>1699.0</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s" s="0">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B147" t="s" s="0">
-        <v>435</v>
+        <v>524</v>
       </c>
       <c r="C147" t="s" s="0">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D147" t="s" s="0">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E147" t="n" s="0">
-        <v>1770.0</v>
+        <v>1700.0</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s" s="0">
-        <v>480</v>
+        <v>525</v>
       </c>
       <c r="B148" t="s" s="0">
-        <v>481</v>
+        <v>435</v>
       </c>
       <c r="C148" t="s" s="0">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D148" t="s" s="0">
-        <v>92</v>
+        <v>216</v>
       </c>
       <c r="E148" t="n" s="0">
-        <v>1799.0</v>
+        <v>1770.0</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s" s="0">
-        <v>526</v>
+        <v>480</v>
       </c>
       <c r="B149" t="s" s="0">
-        <v>527</v>
+        <v>481</v>
       </c>
       <c r="C149" t="s" s="0">
-        <v>528</v>
+        <v>217</v>
       </c>
       <c r="D149" t="s" s="0">
-        <v>529</v>
+        <v>92</v>
       </c>
       <c r="E149" t="n" s="0">
         <v>1799.0</v>
@@ -5090,50 +5117,50 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s" s="0">
-        <v>499</v>
+        <v>526</v>
       </c>
       <c r="B150" t="s" s="0">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C150" t="s" s="0">
-        <v>218</v>
+        <v>698</v>
       </c>
       <c r="D150" t="s" s="0">
-        <v>219</v>
+        <v>529</v>
       </c>
       <c r="E150" t="n" s="0">
-        <v>2100.0</v>
+        <v>1799.0</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s" s="0">
-        <v>474</v>
+        <v>499</v>
       </c>
       <c r="B151" t="s" s="0">
-        <v>475</v>
+        <v>530</v>
       </c>
       <c r="C151" t="s" s="0">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D151" t="s" s="0">
-        <v>76</v>
+        <v>219</v>
       </c>
       <c r="E151" t="n" s="0">
-        <v>2299.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B152" t="s" s="0">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C152" t="s" s="0">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D152" t="s" s="0">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E152" t="n" s="0">
         <v>2299.0</v>
@@ -5147,13 +5174,13 @@
         <v>481</v>
       </c>
       <c r="C153" t="s" s="0">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D153" t="s" s="0">
         <v>92</v>
       </c>
       <c r="E153" t="n" s="0">
-        <v>2499.0</v>
+        <v>2299.0</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
@@ -5198,7 +5225,7 @@
         <v>481</v>
       </c>
       <c r="C156" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D156" t="s" s="0">
         <v>92</v>
@@ -5209,35 +5236,52 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s" s="0">
-        <v>531</v>
+        <v>480</v>
       </c>
       <c r="B157" t="s" s="0">
-        <v>435</v>
+        <v>481</v>
       </c>
       <c r="C157" t="s" s="0">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D157" t="s" s="0">
-        <v>227</v>
+        <v>92</v>
       </c>
       <c r="E157" t="n" s="0">
-        <v>2950.0</v>
+        <v>2499.0</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s" s="0">
+        <v>531</v>
+      </c>
+      <c r="B158" t="s" s="0">
+        <v>435</v>
+      </c>
+      <c r="C158" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="D158" t="s" s="0">
+        <v>227</v>
+      </c>
+      <c r="E158" t="n" s="0">
+        <v>2950.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="0">
         <v>597</v>
       </c>
-      <c r="B158" t="s" s="0">
+      <c r="B159" t="s" s="0">
         <v>568</v>
       </c>
-      <c r="C158" t="s" s="0">
+      <c r="C159" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="D158" t="s" s="0">
+      <c r="D159" t="s" s="0">
         <v>229</v>
       </c>
-      <c r="E158" t="n" s="0">
+      <c r="E159" t="n" s="0">
         <v>3000.0</v>
       </c>
     </row>
@@ -5328,10 +5372,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>243</v>
@@ -5342,10 +5386,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>243</v>
@@ -5608,10 +5652,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>537</v>
+        <v>241</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>289</v>
@@ -5622,10 +5666,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>241</v>
+        <v>537</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>289</v>
@@ -5989,7 +6033,7 @@
         <v>343</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C53" t="s" s="0">
         <v>345</v>
@@ -6003,7 +6047,7 @@
         <v>343</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C54" t="s" s="0">
         <v>345</v>
@@ -6017,7 +6061,7 @@
         <v>343</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C55" t="s" s="0">
         <v>345</v>
@@ -6098,10 +6142,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>421</v>
+        <v>356</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>422</v>
+        <v>357</v>
       </c>
       <c r="C61" t="s" s="0">
         <v>237</v>
@@ -6112,10 +6156,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>356</v>
+        <v>421</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>357</v>
+        <v>422</v>
       </c>
       <c r="C62" t="s" s="0">
         <v>237</v>
@@ -6352,10 +6396,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>384</v>
@@ -6363,10 +6407,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>384</v>
@@ -6385,106 +6429,106 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>396</v>
+        <v>569</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>569</v>
+        <v>396</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>534</v>
+        <v>400</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>400</v>
+        <v>534</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>399</v>
+        <v>577</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>380</v>
+        <v>578</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>611</v>
+        <v>399</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>575</v>
+        <v>611</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>576</v>
+        <v>383</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>381</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>543</v>
+        <v>575</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>383</v>
+        <v>576</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>577</v>
+        <v>543</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>578</v>
+        <v>383</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>384</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>535</v>
+        <v>570</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>380</v>
@@ -6495,7 +6539,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>570</v>
+        <v>535</v>
       </c>
       <c r="B23" t="s" s="0">
         <v>380</v>
@@ -6528,10 +6572,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>571</v>
+        <v>544</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>572</v>
+        <v>545</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>381</v>
@@ -6539,24 +6583,24 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>544</v>
+        <v>405</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>545</v>
+        <v>406</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>381</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>405</v>
+        <v>571</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>406</v>
+        <v>572</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>397</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29">

</xml_diff>

<commit_message>
Made changes in Login and Logout workflow
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ExcelData.xlsx
+++ b/src/test/resources/testdata/ExcelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25971" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29037" uniqueCount="704">
   <si>
     <t>Start Date</t>
   </si>
@@ -2199,6 +2199,21 @@
   </si>
   <si>
     <t>Waterfall Hike</t>
+  </si>
+  <si>
+    <t>2025-07-17T19:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T19:00:00</t>
+  </si>
+  <si>
+    <t>18 Jul - 18 Aug, 3PM</t>
+  </si>
+  <si>
+    <t>2025-07-17T19:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-17T19:30:00</t>
   </si>
 </sst>
 </file>
@@ -2703,7 +2718,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>432</v>
+        <v>547</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>458</v>
@@ -2720,10 +2735,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>690</v>
+        <v>567</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>691</v>
+        <v>546</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>16</v>
@@ -2873,10 +2888,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>690</v>
+        <v>702</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>691</v>
+        <v>703</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>33</v>
@@ -3009,7 +3024,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>432</v>
+        <v>547</v>
       </c>
       <c r="B26" t="s" s="0">
         <v>458</v>
@@ -3349,7 +3364,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>464</v>
+        <v>560</v>
       </c>
       <c r="B46" t="s" s="0">
         <v>465</v>
@@ -3417,7 +3432,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B50" t="s" s="0">
         <v>548</v>
@@ -3474,7 +3489,7 @@
         <v>481</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D53" t="s" s="0">
         <v>92</v>
@@ -3491,7 +3506,7 @@
         <v>481</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s" s="0">
         <v>92</v>
@@ -3723,13 +3738,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D68" t="s" s="0">
         <v>76</v>
@@ -3746,7 +3761,7 @@
         <v>475</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D69" t="s" s="0">
         <v>76</v>
@@ -3757,13 +3772,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B70" t="s" s="0">
         <v>475</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D70" t="s" s="0">
         <v>76</v>
@@ -3780,7 +3795,7 @@
         <v>475</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D71" t="s" s="0">
         <v>76</v>
@@ -3791,13 +3806,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s" s="0">
-        <v>474</v>
+        <v>490</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>475</v>
+        <v>491</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D72" t="s" s="0">
         <v>76</v>
@@ -3814,7 +3829,7 @@
         <v>481</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D73" t="s" s="0">
         <v>92</v>
@@ -3831,7 +3846,7 @@
         <v>481</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D74" t="s" s="0">
         <v>92</v>
@@ -3848,7 +3863,7 @@
         <v>481</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D75" t="s" s="0">
         <v>92</v>
@@ -3865,7 +3880,7 @@
         <v>481</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D76" t="s" s="0">
         <v>92</v>
@@ -3882,7 +3897,7 @@
         <v>481</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="D77" t="s" s="0">
         <v>92</v>
@@ -3899,7 +3914,7 @@
         <v>481</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D78" t="s" s="0">
         <v>92</v>
@@ -3916,7 +3931,7 @@
         <v>481</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D79" t="s" s="0">
         <v>92</v>
@@ -3933,7 +3948,7 @@
         <v>481</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D80" t="s" s="0">
         <v>92</v>
@@ -3950,7 +3965,7 @@
         <v>481</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D81" t="s" s="0">
         <v>92</v>
@@ -3967,7 +3982,7 @@
         <v>481</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D82" t="s" s="0">
         <v>92</v>
@@ -3984,7 +3999,7 @@
         <v>481</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D83" t="s" s="0">
         <v>92</v>
@@ -4001,7 +4016,7 @@
         <v>481</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D84" t="s" s="0">
         <v>92</v>
@@ -4018,7 +4033,7 @@
         <v>481</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D85" t="s" s="0">
         <v>92</v>
@@ -4035,7 +4050,7 @@
         <v>481</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D86" t="s" s="0">
         <v>92</v>
@@ -4052,7 +4067,7 @@
         <v>481</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D87" t="s" s="0">
         <v>92</v>
@@ -4069,7 +4084,7 @@
         <v>481</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D88" t="s" s="0">
         <v>92</v>
@@ -4086,7 +4101,7 @@
         <v>481</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D89" t="s" s="0">
         <v>92</v>
@@ -4120,7 +4135,7 @@
         <v>474</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D91" t="s" s="0">
         <v>94</v>
@@ -4137,7 +4152,7 @@
         <v>474</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D92" t="s" s="0">
         <v>94</v>
@@ -4171,7 +4186,7 @@
         <v>474</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D94" t="s" s="0">
         <v>94</v>
@@ -4188,7 +4203,7 @@
         <v>474</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="D95" t="s" s="0">
         <v>94</v>
@@ -4202,10 +4217,10 @@
         <v>480</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D96" t="s" s="0">
         <v>94</v>
@@ -4219,10 +4234,10 @@
         <v>480</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D97" t="s" s="0">
         <v>94</v>
@@ -4505,13 +4520,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s" s="0">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="B114" t="s" s="0">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="C114" t="s" s="0">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D114" t="s" s="0">
         <v>154</v>
@@ -4539,13 +4554,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s" s="0">
-        <v>510</v>
+        <v>476</v>
       </c>
       <c r="B116" t="s" s="0">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="C116" t="s" s="0">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D116" t="s" s="0">
         <v>154</v>
@@ -4596,7 +4611,7 @@
         <v>481</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D119" t="s" s="0">
         <v>92</v>
@@ -4613,7 +4628,7 @@
         <v>481</v>
       </c>
       <c r="C120" t="s" s="0">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D120" t="s" s="0">
         <v>92</v>
@@ -4630,7 +4645,7 @@
         <v>481</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D121" t="s" s="0">
         <v>92</v>
@@ -4647,7 +4662,7 @@
         <v>481</v>
       </c>
       <c r="C122" t="s" s="0">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D122" t="s" s="0">
         <v>92</v>
@@ -4664,7 +4679,7 @@
         <v>481</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D123" t="s" s="0">
         <v>92</v>
@@ -4698,7 +4713,7 @@
         <v>474</v>
       </c>
       <c r="C125" t="s" s="0">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D125" t="s" s="0">
         <v>94</v>
@@ -4715,7 +4730,7 @@
         <v>474</v>
       </c>
       <c r="C126" t="s" s="0">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D126" t="s" s="0">
         <v>94</v>
@@ -5191,7 +5206,7 @@
         <v>481</v>
       </c>
       <c r="C154" t="s" s="0">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D154" t="s" s="0">
         <v>92</v>
@@ -5208,7 +5223,7 @@
         <v>481</v>
       </c>
       <c r="C155" t="s" s="0">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D155" t="s" s="0">
         <v>92</v>
@@ -5225,7 +5240,7 @@
         <v>481</v>
       </c>
       <c r="C156" t="s" s="0">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D156" t="s" s="0">
         <v>92</v>
@@ -5242,7 +5257,7 @@
         <v>481</v>
       </c>
       <c r="C157" t="s" s="0">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D157" t="s" s="0">
         <v>92</v>
@@ -5316,13 +5331,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>0.0</v>
@@ -5330,13 +5345,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>235</v>
+        <v>601</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>236</v>
+        <v>602</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>237</v>
+        <v>603</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>0.0</v>
@@ -5344,30 +5359,30 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>601</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>602</v>
+        <v>239</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>603</v>
+        <v>240</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>1.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -5386,13 +5401,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>244</v>
+        <v>582</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D7" t="n" s="0">
         <v>49.0</v>
@@ -5400,24 +5415,24 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>582</v>
+        <v>249</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>49.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>251</v>
@@ -5428,10 +5443,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>252</v>
+        <v>409</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>253</v>
+        <v>410</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>251</v>
@@ -5456,13 +5471,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>409</v>
+        <v>255</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>410</v>
+        <v>256</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D12" t="n" s="0">
         <v>99.0</v>
@@ -5470,27 +5485,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>255</v>
+        <v>598</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>99.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>598</v>
+        <v>261</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D14" t="n" s="0">
         <v>100.0</v>
@@ -5498,13 +5513,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D15" t="n" s="0">
         <v>100.0</v>
@@ -5512,13 +5527,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D16" t="n" s="0">
         <v>100.0</v>
@@ -5526,13 +5541,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D17" t="n" s="0">
         <v>100.0</v>
@@ -5540,27 +5555,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>270</v>
+        <v>536</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>100.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>536</v>
+        <v>275</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D19" t="n" s="0">
         <v>149.0</v>
@@ -5568,24 +5583,24 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>149.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>251</v>
@@ -5596,16 +5611,16 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>280</v>
+        <v>583</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="D22" t="n" s="0">
-        <v>150.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -5613,10 +5628,10 @@
         <v>583</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>284</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n" s="0">
         <v>168.0</v>
@@ -5624,13 +5639,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="D24" t="n" s="0">
         <v>168.0</v>
@@ -5638,24 +5653,24 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>583</v>
+        <v>241</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D25" t="n" s="0">
-        <v>168.0</v>
+        <v>169.0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>241</v>
+        <v>537</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>289</v>
@@ -5666,10 +5681,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>537</v>
+        <v>280</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>289</v>
@@ -5680,13 +5695,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D28" t="n" s="0">
         <v>169.0</v>
@@ -5694,13 +5709,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>264</v>
+        <v>294</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D29" t="n" s="0">
         <v>169.0</v>
@@ -5708,44 +5723,44 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D30" t="n" s="0">
-        <v>169.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>297</v>
+        <v>583</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>299</v>
+        <v>8</v>
       </c>
       <c r="D31" t="n" s="0">
-        <v>179.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>583</v>
+        <v>255</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>8</v>
+        <v>302</v>
       </c>
       <c r="D32" t="n" s="0">
-        <v>198.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -5753,10 +5768,10 @@
         <v>255</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="D33" t="n" s="0">
         <v>199.0</v>
@@ -5764,13 +5779,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>255</v>
+        <v>585</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>257</v>
+        <v>306</v>
       </c>
       <c r="D34" t="n" s="0">
         <v>199.0</v>
@@ -5778,13 +5793,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
-        <v>585</v>
+        <v>307</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D35" t="n" s="0">
         <v>199.0</v>
@@ -5792,13 +5807,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="D36" t="n" s="0">
         <v>199.0</v>
@@ -5806,27 +5821,27 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>240</v>
+        <v>316</v>
       </c>
       <c r="D37" t="n" s="0">
-        <v>199.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D38" t="n" s="0">
         <v>200.0</v>
@@ -5834,41 +5849,41 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>264</v>
+        <v>319</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D39" t="n" s="0">
-        <v>200.0</v>
+        <v>219.0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="D40" t="n" s="0">
-        <v>219.0</v>
+        <v>249.0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>274</v>
+        <v>105</v>
       </c>
       <c r="D41" t="n" s="0">
         <v>249.0</v>
@@ -5876,13 +5891,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>324</v>
+        <v>586</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>325</v>
+        <v>247</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>105</v>
+        <v>327</v>
       </c>
       <c r="D42" t="n" s="0">
         <v>249.0</v>
@@ -5890,41 +5905,41 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>586</v>
+        <v>328</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>247</v>
+        <v>329</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D43" t="n" s="0">
-        <v>249.0</v>
+        <v>270.0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s" s="0">
-        <v>328</v>
+        <v>241</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>329</v>
+        <v>411</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>330</v>
+        <v>412</v>
       </c>
       <c r="D44" t="n" s="0">
-        <v>270.0</v>
+        <v>299.0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s" s="0">
-        <v>241</v>
+        <v>331</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>411</v>
+        <v>332</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>412</v>
+        <v>274</v>
       </c>
       <c r="D45" t="n" s="0">
         <v>299.0</v>
@@ -5932,27 +5947,27 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>331</v>
+        <v>538</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>274</v>
+        <v>227</v>
       </c>
       <c r="D46" t="n" s="0">
-        <v>299.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>538</v>
+        <v>334</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>227</v>
+        <v>277</v>
       </c>
       <c r="D47" t="n" s="0">
         <v>300.0</v>
@@ -5960,55 +5975,55 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>277</v>
+        <v>330</v>
       </c>
       <c r="D48" t="n" s="0">
-        <v>300.0</v>
+        <v>320.0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s" s="0">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>330</v>
+        <v>277</v>
       </c>
       <c r="D49" t="n" s="0">
-        <v>320.0</v>
+        <v>349.0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D50" t="n" s="0">
-        <v>349.0</v>
+        <v>399.0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="D51" t="n" s="0">
         <v>399.0</v>
@@ -6016,16 +6031,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>318</v>
+        <v>345</v>
       </c>
       <c r="D52" t="n" s="0">
-        <v>399.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -6033,7 +6048,7 @@
         <v>343</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C53" t="s" s="0">
         <v>345</v>
@@ -6047,7 +6062,7 @@
         <v>343</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C54" t="s" s="0">
         <v>345</v>
@@ -6058,27 +6073,27 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s" s="0">
-        <v>343</v>
+        <v>609</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>344</v>
+        <v>610</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="D55" t="n" s="0">
-        <v>450.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>609</v>
+        <v>348</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>610</v>
+        <v>349</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>364</v>
+        <v>277</v>
       </c>
       <c r="D56" t="n" s="0">
         <v>499.0</v>
@@ -6086,41 +6101,41 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s" s="0">
-        <v>348</v>
+        <v>426</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>349</v>
+        <v>427</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>277</v>
+        <v>428</v>
       </c>
       <c r="D57" t="n" s="0">
-        <v>499.0</v>
+        <v>599.0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s" s="0">
-        <v>426</v>
+        <v>350</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>427</v>
+        <v>351</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>428</v>
+        <v>352</v>
       </c>
       <c r="D58" t="n" s="0">
-        <v>599.0</v>
+        <v>999.0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D59" t="n" s="0">
         <v>999.0</v>
@@ -6128,16 +6143,16 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s" s="0">
-        <v>353</v>
+        <v>421</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>354</v>
+        <v>422</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>355</v>
+        <v>237</v>
       </c>
       <c r="D60" t="n" s="0">
-        <v>999.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -6156,13 +6171,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>421</v>
+        <v>358</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>422</v>
+        <v>359</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>237</v>
+        <v>360</v>
       </c>
       <c r="D62" t="n" s="0">
         <v>1000.0</v>
@@ -6170,100 +6185,100 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>358</v>
+        <v>701</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>360</v>
+        <v>216</v>
       </c>
       <c r="D63" t="n" s="0">
-        <v>1000.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>587</v>
+        <v>362</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>216</v>
+        <v>364</v>
       </c>
       <c r="D64" t="n" s="0">
-        <v>1200.0</v>
+        <v>1499.0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>362</v>
+        <v>264</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>364</v>
+        <v>296</v>
       </c>
       <c r="D65" t="n" s="0">
-        <v>1499.0</v>
+        <v>1999.0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>264</v>
+        <v>366</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>296</v>
+        <v>216</v>
       </c>
       <c r="D66" t="n" s="0">
-        <v>1999.0</v>
+        <v>2010.0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>366</v>
+        <v>423</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>216</v>
+        <v>369</v>
       </c>
       <c r="D67" t="n" s="0">
-        <v>2010.0</v>
+        <v>3000.0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>423</v>
+        <v>370</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D68" t="n" s="0">
-        <v>3000.0</v>
+        <v>5000.0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s" s="0">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="D69" t="n" s="0">
-        <v>5000.0</v>
+        <v>6499.0</v>
       </c>
     </row>
     <row r="70">

</xml_diff>

<commit_message>
Added comments and cleaned unwanted code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ExcelData.xlsx
+++ b/src/test/resources/testdata/ExcelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29037" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31815" uniqueCount="737">
   <si>
     <t>Start Date</t>
   </si>
@@ -2214,6 +2214,105 @@
   </si>
   <si>
     <t>2025-08-17T19:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T08:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T11:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T12:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T12:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T12:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T12:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T11:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T11:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-19T09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-19T09:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-19T09:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-19T23:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-26T22:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-20T05:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-19T04:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-19T21:45:00</t>
+  </si>
+  <si>
+    <t>2025-07-19T08:00:00</t>
+  </si>
+  <si>
+    <t>2025-08-19T14:00:00</t>
+  </si>
+  <si>
+    <t>19 Jul - 18 Aug, 9AM</t>
+  </si>
+  <si>
+    <t>18 Jul, 9PM</t>
+  </si>
+  <si>
+    <t>20 Jul, 6PM</t>
+  </si>
+  <si>
+    <t>Dinner with Strangers | Pune</t>
+  </si>
+  <si>
+    <t>19 Jul - 19 Aug, 9AM</t>
+  </si>
+  <si>
+    <t>2025-08-18T15:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T16:30:00</t>
+  </si>
+  <si>
+    <t>2025-08-18T16:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-20T10:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-25T16:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-18T17:00:00</t>
+  </si>
+  <si>
+    <t>Epitome Pune, Pune</t>
+  </si>
+  <si>
+    <t>27 Jul, 5PM</t>
+  </si>
+  <si>
+    <t>The Underground Marathi Stand-up Comedy Show by Waari | Pune</t>
+  </si>
+  <si>
+    <t>Comedy chi Prayogshala | Marathi Open Mic by Waari Mitra Mandal | Pune</t>
   </si>
 </sst>
 </file>
@@ -2633,10 +2732,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>439</v>
+        <v>567</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>546</v>
+        <v>704</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>5</v>
@@ -2650,10 +2749,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>547</v>
+        <v>440</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>458</v>
+        <v>556</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>7</v>
@@ -2684,10 +2783,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>548</v>
+        <v>705</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>11</v>
@@ -2701,7 +2800,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>438</v>
@@ -2721,7 +2820,7 @@
         <v>547</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>458</v>
+        <v>556</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>15</v>
@@ -2735,10 +2834,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>567</v>
+        <v>608</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>546</v>
+        <v>727</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>16</v>
@@ -2769,7 +2868,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>441</v>
+        <v>706</v>
       </c>
       <c r="B11" t="s" s="0">
         <v>442</v>
@@ -2786,7 +2885,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>438</v>
@@ -2837,10 +2936,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>548</v>
+        <v>705</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>27</v>
@@ -2854,7 +2953,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B16" t="s" s="0">
         <v>438</v>
@@ -2871,10 +2970,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>441</v>
+        <v>706</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>549</v>
+        <v>707</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>31</v>
@@ -2888,10 +2987,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>702</v>
+        <v>608</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>703</v>
+        <v>727</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>33</v>
@@ -2956,7 +3055,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>588</v>
+        <v>486</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>438</v>
@@ -2973,10 +3072,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>554</v>
+        <v>728</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>457</v>
+        <v>729</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>43</v>
@@ -2990,10 +3089,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>554</v>
+        <v>712</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>555</v>
+        <v>713</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>45</v>
@@ -3007,10 +3106,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>547</v>
+        <v>440</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>556</v>
+        <v>714</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>47</v>
@@ -3027,7 +3126,7 @@
         <v>547</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>458</v>
+        <v>556</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>49</v>
@@ -3058,7 +3157,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>461</v>
+        <v>730</v>
       </c>
       <c r="B28" t="s" s="0">
         <v>462</v>
@@ -3075,10 +3174,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>548</v>
+        <v>705</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>52</v>
@@ -3109,10 +3208,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>441</v>
+        <v>706</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>549</v>
+        <v>707</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>55</v>
@@ -3126,10 +3225,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>554</v>
+        <v>712</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>457</v>
+        <v>555</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>56</v>
@@ -3160,7 +3259,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>560</v>
+        <v>451</v>
       </c>
       <c r="B34" t="s" s="0">
         <v>561</v>
@@ -3194,10 +3293,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
-        <v>441</v>
+        <v>706</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>549</v>
+        <v>707</v>
       </c>
       <c r="C36" t="s" s="0">
         <v>64</v>
@@ -3211,10 +3310,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>441</v>
+        <v>706</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>549</v>
+        <v>707</v>
       </c>
       <c r="C37" t="s" s="0">
         <v>65</v>
@@ -3228,7 +3327,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>560</v>
+        <v>451</v>
       </c>
       <c r="B38" t="s" s="0">
         <v>561</v>
@@ -3245,7 +3344,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>467</v>
+        <v>715</v>
       </c>
       <c r="B39" t="s" s="0">
         <v>468</v>
@@ -3262,7 +3361,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B40" t="s" s="0">
         <v>438</v>
@@ -3296,7 +3395,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>559</v>
+        <v>716</v>
       </c>
       <c r="B42" t="s" s="0">
         <v>473</v>
@@ -3313,7 +3412,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>467</v>
+        <v>715</v>
       </c>
       <c r="B43" t="s" s="0">
         <v>468</v>
@@ -3336,7 +3435,7 @@
         <v>475</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D44" t="s" s="0">
         <v>76</v>
@@ -3353,7 +3452,7 @@
         <v>475</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s" s="0">
         <v>76</v>
@@ -3367,7 +3466,7 @@
         <v>560</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>465</v>
+        <v>561</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>78</v>
@@ -3381,7 +3480,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>560</v>
+        <v>451</v>
       </c>
       <c r="B47" t="s" s="0">
         <v>561</v>
@@ -3398,7 +3497,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>476</v>
+        <v>717</v>
       </c>
       <c r="B48" t="s" s="0">
         <v>477</v>
@@ -3435,7 +3534,7 @@
         <v>588</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>548</v>
+        <v>705</v>
       </c>
       <c r="C50" t="s" s="0">
         <v>86</v>
@@ -3449,10 +3548,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>441</v>
+        <v>706</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>549</v>
+        <v>707</v>
       </c>
       <c r="C51" t="s" s="0">
         <v>88</v>
@@ -3489,7 +3588,7 @@
         <v>481</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D53" t="s" s="0">
         <v>92</v>
@@ -3506,7 +3605,7 @@
         <v>481</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D54" t="s" s="0">
         <v>92</v>
@@ -3534,7 +3633,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>482</v>
+        <v>731</v>
       </c>
       <c r="B56" t="s" s="0">
         <v>483</v>
@@ -3574,7 +3673,7 @@
         <v>481</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D58" t="s" s="0">
         <v>92</v>
@@ -3608,7 +3707,7 @@
         <v>481</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D60" t="s" s="0">
         <v>92</v>
@@ -3653,7 +3752,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>486</v>
+        <v>521</v>
       </c>
       <c r="B63" t="s" s="0">
         <v>487</v>
@@ -3687,7 +3786,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>588</v>
+        <v>486</v>
       </c>
       <c r="B65" t="s" s="0">
         <v>438</v>
@@ -3721,7 +3820,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>588</v>
+        <v>486</v>
       </c>
       <c r="B67" t="s" s="0">
         <v>438</v>
@@ -3738,13 +3837,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B68" t="s" s="0">
         <v>475</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D68" t="s" s="0">
         <v>76</v>
@@ -3761,7 +3860,7 @@
         <v>475</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D69" t="s" s="0">
         <v>76</v>
@@ -3772,13 +3871,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s" s="0">
-        <v>474</v>
+        <v>490</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>475</v>
+        <v>491</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D70" t="s" s="0">
         <v>76</v>
@@ -3806,13 +3905,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s" s="0">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D72" t="s" s="0">
         <v>76</v>
@@ -3846,7 +3945,7 @@
         <v>481</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D74" t="s" s="0">
         <v>92</v>
@@ -3863,7 +3962,7 @@
         <v>481</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D75" t="s" s="0">
         <v>92</v>
@@ -3880,7 +3979,7 @@
         <v>481</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D76" t="s" s="0">
         <v>92</v>
@@ -3897,7 +3996,7 @@
         <v>481</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D77" t="s" s="0">
         <v>92</v>
@@ -3914,7 +4013,7 @@
         <v>481</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D78" t="s" s="0">
         <v>92</v>
@@ -3931,7 +4030,7 @@
         <v>481</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D79" t="s" s="0">
         <v>92</v>
@@ -3948,7 +4047,7 @@
         <v>481</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D80" t="s" s="0">
         <v>92</v>
@@ -3965,7 +4064,7 @@
         <v>481</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D81" t="s" s="0">
         <v>92</v>
@@ -3982,7 +4081,7 @@
         <v>481</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D82" t="s" s="0">
         <v>92</v>
@@ -3999,7 +4098,7 @@
         <v>481</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D83" t="s" s="0">
         <v>92</v>
@@ -4016,7 +4115,7 @@
         <v>481</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D84" t="s" s="0">
         <v>92</v>
@@ -4033,7 +4132,7 @@
         <v>481</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D85" t="s" s="0">
         <v>92</v>
@@ -4050,7 +4149,7 @@
         <v>481</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D86" t="s" s="0">
         <v>92</v>
@@ -4084,7 +4183,7 @@
         <v>481</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="D88" t="s" s="0">
         <v>92</v>
@@ -4101,7 +4200,7 @@
         <v>481</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D89" t="s" s="0">
         <v>92</v>
@@ -4118,7 +4217,7 @@
         <v>481</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D90" t="s" s="0">
         <v>92</v>
@@ -4135,7 +4234,7 @@
         <v>474</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D91" t="s" s="0">
         <v>94</v>
@@ -4152,7 +4251,7 @@
         <v>474</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D92" t="s" s="0">
         <v>94</v>
@@ -4166,10 +4265,10 @@
         <v>480</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D93" t="s" s="0">
         <v>94</v>
@@ -4186,7 +4285,7 @@
         <v>474</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D94" t="s" s="0">
         <v>94</v>
@@ -4217,10 +4316,10 @@
         <v>480</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D96" t="s" s="0">
         <v>94</v>
@@ -4248,10 +4347,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s" s="0">
-        <v>541</v>
+        <v>510</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>564</v>
+        <v>718</v>
       </c>
       <c r="C98" t="s" s="0">
         <v>494</v>
@@ -4370,10 +4469,10 @@
         <v>476</v>
       </c>
       <c r="B105" t="s" s="0">
-        <v>477</v>
+        <v>501</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D105" t="s" s="0">
         <v>154</v>
@@ -4387,10 +4486,10 @@
         <v>476</v>
       </c>
       <c r="B106" t="s" s="0">
-        <v>501</v>
+        <v>477</v>
       </c>
       <c r="C106" t="s" s="0">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D106" t="s" s="0">
         <v>154</v>
@@ -4401,7 +4500,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s" s="0">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B107" t="s" s="0">
         <v>503</v>
@@ -4418,7 +4517,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s" s="0">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B108" t="s" s="0">
         <v>503</v>
@@ -4452,13 +4551,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s" s="0">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B110" t="s" s="0">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C110" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D110" t="s" s="0">
         <v>163</v>
@@ -4469,13 +4568,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s" s="0">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="B111" t="s" s="0">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D111" t="s" s="0">
         <v>163</v>
@@ -4537,7 +4636,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s" s="0">
-        <v>512</v>
+        <v>476</v>
       </c>
       <c r="B115" t="s" s="0">
         <v>477</v>
@@ -4611,7 +4710,7 @@
         <v>481</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D119" t="s" s="0">
         <v>92</v>
@@ -4628,7 +4727,7 @@
         <v>481</v>
       </c>
       <c r="C120" t="s" s="0">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D120" t="s" s="0">
         <v>92</v>
@@ -4645,7 +4744,7 @@
         <v>481</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D121" t="s" s="0">
         <v>92</v>
@@ -4679,7 +4778,7 @@
         <v>481</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D123" t="s" s="0">
         <v>92</v>
@@ -4696,7 +4795,7 @@
         <v>481</v>
       </c>
       <c r="C124" t="s" s="0">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D124" t="s" s="0">
         <v>92</v>
@@ -4713,7 +4812,7 @@
         <v>474</v>
       </c>
       <c r="C125" t="s" s="0">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D125" t="s" s="0">
         <v>94</v>
@@ -4730,7 +4829,7 @@
         <v>474</v>
       </c>
       <c r="C126" t="s" s="0">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D126" t="s" s="0">
         <v>94</v>
@@ -4741,10 +4840,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s" s="0">
-        <v>588</v>
+        <v>732</v>
       </c>
       <c r="B127" t="s" s="0">
-        <v>514</v>
+        <v>600</v>
       </c>
       <c r="C127" t="s" s="0">
         <v>183</v>
@@ -4843,7 +4942,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s" s="0">
-        <v>518</v>
+        <v>719</v>
       </c>
       <c r="B133" t="s" s="0">
         <v>519</v>
@@ -4911,10 +5010,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s" s="0">
-        <v>441</v>
+        <v>706</v>
       </c>
       <c r="B137" t="s" s="0">
-        <v>549</v>
+        <v>707</v>
       </c>
       <c r="C137" t="s" s="0">
         <v>197</v>
@@ -4928,10 +5027,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s" s="0">
-        <v>567</v>
+        <v>720</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>546</v>
+        <v>704</v>
       </c>
       <c r="C138" t="s" s="0">
         <v>199</v>
@@ -4945,7 +5044,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s" s="0">
-        <v>518</v>
+        <v>719</v>
       </c>
       <c r="B139" t="s" s="0">
         <v>519</v>
@@ -4996,7 +5095,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s" s="0">
-        <v>443</v>
+        <v>588</v>
       </c>
       <c r="B142" t="s" s="0">
         <v>521</v>
@@ -5019,7 +5118,7 @@
         <v>481</v>
       </c>
       <c r="C143" t="s" s="0">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D143" t="s" s="0">
         <v>92</v>
@@ -5036,7 +5135,7 @@
         <v>481</v>
       </c>
       <c r="C144" t="s" s="0">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D144" t="s" s="0">
         <v>92</v>
@@ -5206,7 +5305,7 @@
         <v>481</v>
       </c>
       <c r="C154" t="s" s="0">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D154" t="s" s="0">
         <v>92</v>
@@ -5223,7 +5322,7 @@
         <v>481</v>
       </c>
       <c r="C155" t="s" s="0">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D155" t="s" s="0">
         <v>92</v>
@@ -5240,7 +5339,7 @@
         <v>481</v>
       </c>
       <c r="C156" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D156" t="s" s="0">
         <v>92</v>
@@ -5257,7 +5356,7 @@
         <v>481</v>
       </c>
       <c r="C157" t="s" s="0">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D157" t="s" s="0">
         <v>92</v>
@@ -5285,10 +5384,10 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="0">
-        <v>597</v>
+        <v>480</v>
       </c>
       <c r="B159" t="s" s="0">
-        <v>568</v>
+        <v>721</v>
       </c>
       <c r="C159" t="s" s="0">
         <v>228</v>
@@ -5307,7 +5406,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -5365,7 +5464,7 @@
         <v>239</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>240</v>
+        <v>733</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>1.0</v>
@@ -5373,10 +5472,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>243</v>
@@ -5387,10 +5486,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>243</v>
@@ -5429,10 +5528,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>251</v>
@@ -5457,10 +5556,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>251</v>
@@ -5527,13 +5626,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>267</v>
+        <v>734</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>268</v>
+        <v>735</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D16" t="n" s="0">
         <v>100.0</v>
@@ -5541,13 +5640,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>270</v>
+        <v>734</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>271</v>
+        <v>736</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D17" t="n" s="0">
         <v>100.0</v>
@@ -5555,97 +5654,97 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>536</v>
+        <v>267</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>149.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>149.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>150.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="D21" t="n" s="0">
-        <v>150.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>583</v>
+        <v>280</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="D22" t="n" s="0">
-        <v>168.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>583</v>
+        <v>278</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>8</v>
+        <v>251</v>
       </c>
       <c r="D23" t="n" s="0">
-        <v>168.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>583</v>
+        <v>722</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D24" t="n" s="0">
         <v>168.0</v>
@@ -5653,38 +5752,38 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>241</v>
+        <v>587</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>289</v>
+        <v>8</v>
       </c>
       <c r="D25" t="n" s="0">
-        <v>169.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>537</v>
+        <v>722</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D26" t="n" s="0">
-        <v>169.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>280</v>
+        <v>241</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>289</v>
@@ -5695,13 +5794,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>264</v>
+        <v>723</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D28" t="n" s="0">
         <v>169.0</v>
@@ -5709,13 +5808,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D29" t="n" s="0">
         <v>169.0</v>
@@ -5723,69 +5822,69 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
-        <v>297</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D30" t="n" s="0">
-        <v>179.0</v>
+        <v>169.0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>583</v>
+        <v>294</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>8</v>
+        <v>296</v>
       </c>
       <c r="D31" t="n" s="0">
-        <v>198.0</v>
+        <v>169.0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D32" t="n" s="0">
-        <v>199.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s" s="0">
-        <v>255</v>
+        <v>722</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>257</v>
+        <v>8</v>
       </c>
       <c r="D33" t="n" s="0">
-        <v>199.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>585</v>
+        <v>255</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D34" t="n" s="0">
         <v>199.0</v>
@@ -5793,13 +5892,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
-        <v>307</v>
+        <v>255</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>309</v>
+        <v>257</v>
       </c>
       <c r="D35" t="n" s="0">
         <v>199.0</v>
@@ -5807,13 +5906,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
-        <v>310</v>
+        <v>585</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>240</v>
+        <v>306</v>
       </c>
       <c r="D36" t="n" s="0">
         <v>199.0</v>
@@ -5821,83 +5920,83 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D37" t="n" s="0">
-        <v>200.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>264</v>
+        <v>310</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>318</v>
+        <v>240</v>
       </c>
       <c r="D38" t="n" s="0">
-        <v>200.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D39" t="n" s="0">
-        <v>219.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>322</v>
+        <v>264</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="D40" t="n" s="0">
-        <v>249.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>105</v>
+        <v>321</v>
       </c>
       <c r="D41" t="n" s="0">
-        <v>249.0</v>
+        <v>219.0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>586</v>
+        <v>322</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>247</v>
+        <v>323</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>327</v>
+        <v>274</v>
       </c>
       <c r="D42" t="n" s="0">
         <v>249.0</v>
@@ -5905,156 +6004,156 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>330</v>
+        <v>105</v>
       </c>
       <c r="D43" t="n" s="0">
-        <v>270.0</v>
+        <v>249.0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s" s="0">
-        <v>241</v>
+        <v>586</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>411</v>
+        <v>247</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>412</v>
+        <v>327</v>
       </c>
       <c r="D44" t="n" s="0">
-        <v>299.0</v>
+        <v>249.0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s" s="0">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>274</v>
+        <v>330</v>
       </c>
       <c r="D45" t="n" s="0">
-        <v>299.0</v>
+        <v>270.0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>538</v>
+        <v>241</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>333</v>
+        <v>411</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>227</v>
+        <v>412</v>
       </c>
       <c r="D46" t="n" s="0">
-        <v>300.0</v>
+        <v>299.0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D47" t="n" s="0">
-        <v>300.0</v>
+        <v>299.0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>336</v>
+        <v>538</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>330</v>
+        <v>227</v>
       </c>
       <c r="D48" t="n" s="0">
-        <v>320.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s" s="0">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>277</v>
       </c>
       <c r="D49" t="n" s="0">
-        <v>349.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>274</v>
+        <v>330</v>
       </c>
       <c r="D50" t="n" s="0">
-        <v>399.0</v>
+        <v>320.0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="D51" t="n" s="0">
-        <v>399.0</v>
+        <v>349.0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s" s="0">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>345</v>
+        <v>274</v>
       </c>
       <c r="D52" t="n" s="0">
-        <v>450.0</v>
+        <v>399.0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s" s="0">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="D53" t="n" s="0">
-        <v>450.0</v>
+        <v>399.0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -6073,225 +6172,253 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s" s="0">
-        <v>609</v>
+        <v>343</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>610</v>
+        <v>346</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="D55" t="n" s="0">
-        <v>499.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>277</v>
+        <v>345</v>
       </c>
       <c r="D56" t="n" s="0">
-        <v>499.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s" s="0">
-        <v>426</v>
+        <v>609</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>427</v>
+        <v>610</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>428</v>
+        <v>364</v>
       </c>
       <c r="D57" t="n" s="0">
-        <v>599.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s" s="0">
-        <v>350</v>
+        <v>724</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>351</v>
+        <v>725</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>352</v>
+        <v>243</v>
       </c>
       <c r="D58" t="n" s="0">
-        <v>999.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>355</v>
+        <v>277</v>
       </c>
       <c r="D59" t="n" s="0">
-        <v>999.0</v>
+        <v>499.0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s" s="0">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>237</v>
+        <v>428</v>
       </c>
       <c r="D60" t="n" s="0">
-        <v>1000.0</v>
+        <v>599.0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>237</v>
+        <v>352</v>
       </c>
       <c r="D61" t="n" s="0">
-        <v>1000.0</v>
+        <v>999.0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D62" t="n" s="0">
-        <v>1000.0</v>
+        <v>999.0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>701</v>
+        <v>356</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="D63" t="n" s="0">
-        <v>1200.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>362</v>
+        <v>421</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>363</v>
+        <v>422</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>364</v>
+        <v>237</v>
       </c>
       <c r="D64" t="n" s="0">
-        <v>1499.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>264</v>
+        <v>358</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>296</v>
+        <v>360</v>
       </c>
       <c r="D65" t="n" s="0">
-        <v>1999.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>366</v>
+        <v>726</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C66" t="s" s="0">
         <v>216</v>
       </c>
       <c r="D66" t="n" s="0">
-        <v>2010.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>423</v>
+        <v>362</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D67" t="n" s="0">
-        <v>3000.0</v>
+        <v>1499.0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>370</v>
+        <v>264</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>372</v>
+        <v>296</v>
       </c>
       <c r="D68" t="n" s="0">
-        <v>5000.0</v>
+        <v>1999.0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s" s="0">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>375</v>
+        <v>216</v>
       </c>
       <c r="D69" t="n" s="0">
-        <v>6499.0</v>
+        <v>2010.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
+        <v>423</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>368</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="D70" t="n" s="0">
+        <v>3000.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>370</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>371</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="D71" t="n" s="0">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="B70" t="s" s="0">
+      <c r="B72" t="s" s="0">
         <v>374</v>
       </c>
-      <c r="C70" t="s" s="0">
+      <c r="C72" t="s" s="0">
         <v>375</v>
       </c>
-      <c r="D70" t="n" s="0">
+      <c r="D72" t="n" s="0">
         <v>6499.0</v>
       </c>
     </row>
@@ -6356,7 +6483,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>380</v>
@@ -6367,7 +6494,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>380</v>
@@ -6411,13 +6538,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>392</v>
+        <v>534</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -6433,43 +6560,43 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>580</v>
+        <v>399</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>569</v>
+        <v>396</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>380</v>
+        <v>401</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>397</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>400</v>
+        <v>577</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>401</v>
+        <v>578</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>384</v>
@@ -6477,54 +6604,54 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>534</v>
+        <v>543</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>381</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>578</v>
+        <v>383</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>384</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>399</v>
+        <v>535</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>380</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>389</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>611</v>
+        <v>575</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>383</v>
+        <v>576</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>576</v>
+        <v>383</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>381</v>
@@ -6532,10 +6659,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>543</v>
+        <v>570</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>403</v>
@@ -6543,10 +6670,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>570</v>
+        <v>542</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>403</v>
@@ -6554,68 +6681,68 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>535</v>
+        <v>581</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>383</v>
+        <v>545</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>383</v>
+        <v>572</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>544</v>
+        <v>573</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>545</v>
+        <v>574</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>381</v>
+        <v>397</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>405</v>
+        <v>611</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>381</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29">

</xml_diff>